<commit_message>
feat: last commit of the week
</commit_message>
<xml_diff>
--- a/__docs/diary.xlsx
+++ b/__docs/diary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gimesia\Documents\PROJEKT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gimesia\Documents\PROJEKT\zebrafish_pipenv\__docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>Felmerült problémák:</t>
   </si>
@@ -836,6 +836,54 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -847,54 +895,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1176,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY30"/>
+  <dimension ref="A1:AY20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1420,11 +1420,11 @@
         <v>0.79583333333333339</v>
       </c>
       <c r="E3" s="57">
-        <v>0.75</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="F3" s="63">
         <f>AVERAGE(B3:E3)</f>
-        <v>0.79270833333333335</v>
+        <v>0.78749999999999998</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="16"/>
@@ -1488,11 +1488,11 @@
       </c>
       <c r="E4" s="67">
         <f>E3-E2</f>
-        <v>0.40138888888888885</v>
+        <v>0.38055555555555548</v>
       </c>
       <c r="F4" s="63">
         <f>AVERAGE(B4:E4)</f>
-        <v>0.39756944444444442</v>
+        <v>0.3923611111111111</v>
       </c>
       <c r="G4" s="67">
         <f t="shared" ref="G4:AW4" si="0">G3-G2</f>
@@ -1838,7 +1838,7 @@
       <c r="D11" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="71" t="s">
         <v>44</v>
       </c>
       <c r="F11" s="64"/>
@@ -1864,7 +1864,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="22"/>
-      <c r="E12" s="75" t="s">
+      <c r="E12" s="71" t="s">
         <v>45</v>
       </c>
       <c r="F12" s="64"/>
@@ -2023,286 +2023,42 @@
       <c r="S18" s="42"/>
       <c r="T18" s="43"/>
     </row>
-    <row r="19" spans="1:20" s="40" customFormat="1" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="59"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="39"/>
-    </row>
-    <row r="20" spans="1:20" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
-      <c r="B20" s="21" t="s">
+    <row r="19" spans="1:20" s="49" customFormat="1" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="46">
+        <v>3.5</v>
+      </c>
+      <c r="C19" s="47">
         <v>4</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="22"/>
-      <c r="T20" s="27"/>
-    </row>
-    <row r="21" spans="1:20" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="23"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="22"/>
-      <c r="S21" s="22"/>
-      <c r="T21" s="27"/>
-    </row>
-    <row r="22" spans="1:20" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="28"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="22"/>
-      <c r="T22" s="27"/>
-    </row>
-    <row r="23" spans="1:20" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="22"/>
-      <c r="S23" s="22"/>
-      <c r="T23" s="27"/>
-    </row>
-    <row r="24" spans="1:20" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="28"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="22"/>
-      <c r="S24" s="22"/>
-      <c r="T24" s="27"/>
-    </row>
-    <row r="25" spans="1:20" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
-      <c r="R25" s="22"/>
-      <c r="S25" s="22"/>
-      <c r="T25" s="27"/>
-    </row>
-    <row r="26" spans="1:20" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="28"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
-      <c r="T26" s="27"/>
-    </row>
-    <row r="27" spans="1:20" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="28"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="22"/>
-      <c r="S27" s="22"/>
-      <c r="T27" s="27"/>
-    </row>
-    <row r="28" spans="1:20" s="44" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="32"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="42"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="42"/>
-      <c r="N28" s="42"/>
-      <c r="O28" s="42"/>
-      <c r="P28" s="42"/>
-      <c r="Q28" s="42"/>
-      <c r="R28" s="42"/>
-      <c r="S28" s="42"/>
-      <c r="T28" s="43"/>
-    </row>
-    <row r="29" spans="1:20" s="49" customFormat="1" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="46">
+      <c r="D19" s="47">
+        <v>1.5</v>
+      </c>
+      <c r="E19" s="61">
         <v>3.5</v>
       </c>
-      <c r="C29" s="47">
-        <v>4</v>
-      </c>
-      <c r="D29" s="47">
-        <v>1.5</v>
-      </c>
-      <c r="E29" s="61"/>
-      <c r="F29" s="65">
-        <f>AVERAGE(B29:E29)</f>
-        <v>3</v>
-      </c>
-      <c r="G29" s="46"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="47"/>
-      <c r="P29" s="47"/>
-      <c r="Q29" s="47"/>
-      <c r="R29" s="47"/>
-      <c r="S29" s="47"/>
-      <c r="T29" s="48"/>
-    </row>
-    <row r="30" spans="1:20" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="F19" s="65">
+        <f>AVERAGE(B19:E19)</f>
+        <v>3.125</v>
+      </c>
+      <c r="G19" s="46"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="47"/>
+      <c r="Q19" s="47"/>
+      <c r="R19" s="47"/>
+      <c r="S19" s="47"/>
+      <c r="T19" s="48"/>
+    </row>
+    <row r="20" spans="1:20" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2319,7 +2075,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.33203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="85" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="81" customWidth="1"/>
     <col min="2" max="2" width="10.109375" style="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" style="50" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.88671875" style="50" bestFit="1" customWidth="1"/>
@@ -2328,227 +2084,227 @@
     <col min="7" max="16384" width="32.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="76" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79"/>
-      <c r="B1" s="77">
+    <row r="1" spans="1:49" s="72" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="75"/>
+      <c r="B1" s="73">
         <v>44753</v>
       </c>
-      <c r="C1" s="77">
+      <c r="C1" s="73">
         <v>44754</v>
       </c>
-      <c r="D1" s="77">
+      <c r="D1" s="73">
         <v>44755</v>
       </c>
-      <c r="E1" s="77">
+      <c r="E1" s="73">
         <v>44756</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="76">
+      <c r="G1" s="72">
         <v>44760</v>
       </c>
-      <c r="H1" s="76">
+      <c r="H1" s="72">
         <v>44761</v>
       </c>
-      <c r="I1" s="76">
+      <c r="I1" s="72">
         <v>44762</v>
       </c>
-      <c r="J1" s="76">
+      <c r="J1" s="72">
         <v>44763</v>
       </c>
-      <c r="K1" s="76">
+      <c r="K1" s="72">
         <v>44764</v>
       </c>
-      <c r="L1" s="76">
+      <c r="L1" s="72">
         <v>44765</v>
       </c>
-      <c r="M1" s="76">
+      <c r="M1" s="72">
         <v>44766</v>
       </c>
-      <c r="N1" s="76">
+      <c r="N1" s="72">
         <v>44767</v>
       </c>
-      <c r="O1" s="76">
+      <c r="O1" s="72">
         <v>44768</v>
       </c>
-      <c r="P1" s="76">
+      <c r="P1" s="72">
         <v>44769</v>
       </c>
-      <c r="Q1" s="76">
+      <c r="Q1" s="72">
         <v>44770</v>
       </c>
-      <c r="R1" s="76">
+      <c r="R1" s="72">
         <v>44771</v>
       </c>
-      <c r="S1" s="76">
+      <c r="S1" s="72">
         <v>44772</v>
       </c>
-      <c r="T1" s="76">
+      <c r="T1" s="72">
         <v>44773</v>
       </c>
-      <c r="U1" s="76">
+      <c r="U1" s="72">
         <v>44774</v>
       </c>
-      <c r="V1" s="76">
+      <c r="V1" s="72">
         <v>44775</v>
       </c>
-      <c r="W1" s="76">
+      <c r="W1" s="72">
         <v>44776</v>
       </c>
-      <c r="X1" s="76">
+      <c r="X1" s="72">
         <v>44777</v>
       </c>
-      <c r="Y1" s="76">
+      <c r="Y1" s="72">
         <v>44778</v>
       </c>
-      <c r="Z1" s="76">
+      <c r="Z1" s="72">
         <v>44779</v>
       </c>
-      <c r="AA1" s="76">
+      <c r="AA1" s="72">
         <v>44780</v>
       </c>
-      <c r="AB1" s="76">
+      <c r="AB1" s="72">
         <v>44781</v>
       </c>
-      <c r="AC1" s="76">
+      <c r="AC1" s="72">
         <v>44782</v>
       </c>
-      <c r="AD1" s="76">
+      <c r="AD1" s="72">
         <v>44783</v>
       </c>
-      <c r="AE1" s="76">
+      <c r="AE1" s="72">
         <v>44784</v>
       </c>
-      <c r="AF1" s="76">
+      <c r="AF1" s="72">
         <v>44785</v>
       </c>
-      <c r="AG1" s="76">
+      <c r="AG1" s="72">
         <v>44786</v>
       </c>
-      <c r="AH1" s="76">
+      <c r="AH1" s="72">
         <v>44787</v>
       </c>
-      <c r="AI1" s="76">
+      <c r="AI1" s="72">
         <v>44788</v>
       </c>
-      <c r="AJ1" s="76">
+      <c r="AJ1" s="72">
         <v>44789</v>
       </c>
-      <c r="AK1" s="76">
+      <c r="AK1" s="72">
         <v>44790</v>
       </c>
-      <c r="AL1" s="76">
+      <c r="AL1" s="72">
         <v>44791</v>
       </c>
-      <c r="AM1" s="76">
+      <c r="AM1" s="72">
         <v>44792</v>
       </c>
-      <c r="AN1" s="76">
+      <c r="AN1" s="72">
         <v>44793</v>
       </c>
-      <c r="AO1" s="76">
+      <c r="AO1" s="72">
         <v>44794</v>
       </c>
-      <c r="AP1" s="76">
+      <c r="AP1" s="72">
         <v>44795</v>
       </c>
-      <c r="AQ1" s="76">
+      <c r="AQ1" s="72">
         <v>44796</v>
       </c>
-      <c r="AR1" s="76">
+      <c r="AR1" s="72">
         <v>44797</v>
       </c>
-      <c r="AS1" s="76">
+      <c r="AS1" s="72">
         <v>44798</v>
       </c>
-      <c r="AT1" s="76">
+      <c r="AT1" s="72">
         <v>44799</v>
       </c>
-      <c r="AU1" s="76">
+      <c r="AU1" s="72">
         <v>44800</v>
       </c>
-      <c r="AV1" s="76">
+      <c r="AV1" s="72">
         <v>44801</v>
       </c>
-      <c r="AW1" s="76">
+      <c r="AW1" s="72">
         <v>44802</v>
       </c>
     </row>
     <row r="2" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="87">
+      <c r="A2" s="83">
         <v>0.33333333333333331</v>
       </c>
       <c r="B2" s="53"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="88"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="84"/>
     </row>
     <row r="3" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="84">
+      <c r="A3" s="80">
         <v>0.35416666666666669</v>
       </c>
-      <c r="C3" s="81"/>
+      <c r="C3" s="77"/>
       <c r="D3" s="51" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="89"/>
+      <c r="F3" s="85"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="84">
+      <c r="A4" s="80">
         <v>0.375</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="74" t="s">
+      <c r="C4" s="77"/>
+      <c r="D4" s="90" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="89"/>
+      <c r="F4" s="85"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="84">
+      <c r="A5" s="80">
         <v>0.39583333333333298</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="74"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="90"/>
       <c r="E5" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="89"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="84">
+      <c r="A6" s="80">
         <v>0.41666666666666702</v>
       </c>
       <c r="C6" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="74"/>
-      <c r="E6" s="71" t="s">
+      <c r="D6" s="90"/>
+      <c r="E6" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="89"/>
+      <c r="F6" s="85"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="84">
+      <c r="A7" s="80">
         <v>0.4375</v>
       </c>
       <c r="C7" s="51" t="s">
@@ -2557,174 +2313,174 @@
       <c r="D7" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="73"/>
-      <c r="F7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="85"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="84">
+      <c r="A8" s="80">
         <v>0.45833333333333298</v>
       </c>
       <c r="C8" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="71" t="s">
+      <c r="D8" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="73"/>
-      <c r="F8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="85"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="84">
+      <c r="A9" s="80">
         <v>0.47916666666666702</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="85"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="84">
+      <c r="A10" s="80">
         <v>0.5</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="71" t="s">
+      <c r="C10" s="90"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="89"/>
+      <c r="F10" s="85"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="84">
+      <c r="A11" s="80">
         <v>0.52083333333333304</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="89"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="85"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="84">
+      <c r="A12" s="80">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C12" s="74" t="s">
+      <c r="C12" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="72"/>
+      <c r="D12" s="88"/>
       <c r="E12" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="89"/>
+      <c r="F12" s="85"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="84">
+      <c r="A13" s="80">
         <v>0.5625</v>
       </c>
-      <c r="C13" s="74"/>
-      <c r="D13" s="71" t="s">
+      <c r="C13" s="90"/>
+      <c r="D13" s="87" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="89"/>
+      <c r="F13" s="85"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="84">
+      <c r="A14" s="80">
         <v>0.58333333333333304</v>
       </c>
-      <c r="C14" s="74" t="s">
+      <c r="C14" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="72"/>
-      <c r="E14" s="71" t="s">
+      <c r="D14" s="88"/>
+      <c r="E14" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="89"/>
+      <c r="F14" s="85"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="84">
+      <c r="A15" s="80">
         <v>0.60416666666666696</v>
       </c>
-      <c r="C15" s="74"/>
-      <c r="D15" s="71" t="s">
+      <c r="C15" s="90"/>
+      <c r="D15" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="72"/>
-      <c r="F15" s="89"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="85"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="84">
+      <c r="A16" s="80">
         <v>0.625</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="C16" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="72"/>
-      <c r="E16" s="71" t="s">
+      <c r="D16" s="88"/>
+      <c r="E16" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="89"/>
+      <c r="F16" s="85"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="84">
+      <c r="A17" s="80">
         <v>0.64583333333333404</v>
       </c>
-      <c r="C17" s="74"/>
-      <c r="D17" s="71" t="s">
+      <c r="C17" s="90"/>
+      <c r="D17" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="72"/>
-      <c r="F17" s="89"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="85"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="84">
+      <c r="A18" s="80">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C18" s="74"/>
-      <c r="D18" s="72"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="88"/>
       <c r="E18" s="51"/>
-      <c r="F18" s="89"/>
+      <c r="F18" s="85"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="84">
+      <c r="A19" s="80">
         <v>0.6875</v>
       </c>
       <c r="C19" s="51" t="s">
@@ -2734,139 +2490,139 @@
         <v>35</v>
       </c>
       <c r="E19" s="51"/>
-      <c r="F19" s="89"/>
+      <c r="F19" s="85"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="84">
+      <c r="A20" s="80">
         <v>0.70833333333333404</v>
       </c>
       <c r="C20" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="71" t="s">
+      <c r="D20" s="87" t="s">
         <v>29</v>
       </c>
       <c r="E20" s="51"/>
-      <c r="F20" s="89"/>
+      <c r="F20" s="85"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="84">
+      <c r="A21" s="80">
         <v>0.72916666666666696</v>
       </c>
-      <c r="C21" s="74" t="s">
+      <c r="C21" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="72"/>
+      <c r="D21" s="88"/>
       <c r="E21" s="51"/>
-      <c r="F21" s="89"/>
+      <c r="F21" s="85"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="84">
+      <c r="A22" s="80">
         <v>0.75</v>
       </c>
-      <c r="C22" s="74"/>
+      <c r="C22" s="90"/>
       <c r="D22" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="83"/>
-      <c r="F22" s="89"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="85"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="84">
+      <c r="A23" s="80">
         <v>0.77083333333333404</v>
       </c>
-      <c r="C23" s="74"/>
+      <c r="C23" s="90"/>
       <c r="D23" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="83"/>
-      <c r="F23" s="89"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="85"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="84">
+      <c r="A24" s="80">
         <v>0.79166666666666696</v>
       </c>
       <c r="C24" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="83"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="89"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="85"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="84">
+      <c r="A25" s="80">
         <v>0.8125</v>
       </c>
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="89"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="85"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="84">
+      <c r="A26" s="80">
         <v>0.83333333333333304</v>
       </c>
-      <c r="C26" s="83"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="89"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="85"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="84">
+      <c r="A27" s="80">
         <v>0.85416666666666596</v>
       </c>
-      <c r="C27" s="83"/>
-      <c r="D27" s="83"/>
-      <c r="E27" s="83"/>
-      <c r="F27" s="89"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="85"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="86">
+      <c r="A28" s="82">
         <v>0.874999999999999</v>
       </c>
-      <c r="C28" s="83"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="89"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="79"/>
+      <c r="E28" s="79"/>
+      <c r="F28" s="85"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F29" s="90"/>
+      <c r="F29" s="86"/>
     </row>
     <row r="30" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F30" s="90"/>
+      <c r="F30" s="86"/>
     </row>
     <row r="31" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F31" s="90"/>
+      <c r="F31" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
refactor: created src folder
</commit_message>
<xml_diff>
--- a/__docs/diary.xlsx
+++ b/__docs/diary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Felmerült problémák:</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>Mapping Toolbox is kell a MATLAB progi működéséhez</t>
+  </si>
+  <si>
+    <t>getInnerROI.m-nél tartottam</t>
+  </si>
+  <si>
+    <t>megpróbálom megcsinálni, hogy fusson minden modul, ha nem jól akkor is</t>
+  </si>
+  <si>
+    <t>create_circle_mask.py</t>
   </si>
 </sst>
 </file>
@@ -626,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -884,17 +893,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1178,17 +1193,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="66.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55" style="66"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="3" max="3" width="72.44140625" customWidth="1"/>
+    <col min="4" max="4" width="80.44140625" customWidth="1"/>
+    <col min="5" max="5" width="66.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="66" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="55" style="2"/>
     <col min="18" max="20" width="55" style="2"/>
     <col min="25" max="30" width="55" style="2"/>
@@ -1362,7 +1379,9 @@
         <f>AVERAGE(B2:E2)</f>
         <v>0.39513888888888893</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2" s="12">
+        <v>0.35416666666666669</v>
+      </c>
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
@@ -1496,7 +1515,7 @@
       </c>
       <c r="G4" s="67">
         <f t="shared" ref="G4:AW4" si="0">G3-G2</f>
-        <v>0</v>
+        <v>-0.35416666666666669</v>
       </c>
       <c r="H4" s="67">
         <f t="shared" si="0"/>
@@ -1682,7 +1701,9 @@
         <v>38</v>
       </c>
       <c r="F5" s="64"/>
-      <c r="G5" s="18"/>
+      <c r="G5" s="18" t="s">
+        <v>51</v>
+      </c>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
@@ -1708,7 +1729,9 @@
         <v>39</v>
       </c>
       <c r="F6" s="64"/>
-      <c r="G6" s="18"/>
+      <c r="G6" s="18" t="s">
+        <v>52</v>
+      </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
@@ -2069,8 +2092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.33203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2240,6 +2263,7 @@
       <c r="D2" s="78"/>
       <c r="E2" s="78"/>
       <c r="F2" s="84"/>
+      <c r="G2" s="92"/>
     </row>
     <row r="3" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="80">
@@ -2253,7 +2277,9 @@
         <v>28</v>
       </c>
       <c r="F3" s="85"/>
-      <c r="G3" s="3"/>
+      <c r="G3" s="87" t="s">
+        <v>28</v>
+      </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
@@ -2262,14 +2288,16 @@
         <v>0.375</v>
       </c>
       <c r="C4" s="77"/>
-      <c r="D4" s="90" t="s">
+      <c r="D4" s="91" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="85"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
@@ -2278,12 +2306,14 @@
         <v>0.39583333333333298</v>
       </c>
       <c r="C5" s="77"/>
-      <c r="D5" s="90"/>
+      <c r="D5" s="91"/>
       <c r="E5" s="51" t="s">
         <v>41</v>
       </c>
       <c r="F5" s="85"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
@@ -2294,12 +2324,14 @@
       <c r="C6" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="90"/>
-      <c r="E6" s="87" t="s">
+      <c r="D6" s="91"/>
+      <c r="E6" s="88" t="s">
         <v>46</v>
       </c>
       <c r="F6" s="85"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
@@ -2326,7 +2358,7 @@
       <c r="C8" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="87" t="s">
+      <c r="D8" s="88" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="89"/>
@@ -2339,11 +2371,11 @@
       <c r="A9" s="80">
         <v>0.47916666666666702</v>
       </c>
-      <c r="C9" s="90" t="s">
+      <c r="C9" s="91" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="89"/>
-      <c r="E9" s="88"/>
+      <c r="E9" s="90"/>
       <c r="F9" s="85"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -2353,9 +2385,9 @@
       <c r="A10" s="80">
         <v>0.5</v>
       </c>
-      <c r="C10" s="90"/>
+      <c r="C10" s="91"/>
       <c r="D10" s="89"/>
-      <c r="E10" s="87" t="s">
+      <c r="E10" s="88" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="85"/>
@@ -2367,9 +2399,9 @@
       <c r="A11" s="80">
         <v>0.52083333333333304</v>
       </c>
-      <c r="C11" s="90"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="89"/>
-      <c r="E11" s="88"/>
+      <c r="E11" s="90"/>
       <c r="F11" s="85"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2379,10 +2411,10 @@
       <c r="A12" s="80">
         <v>0.54166666666666696</v>
       </c>
-      <c r="C12" s="90" t="s">
+      <c r="C12" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="88"/>
+      <c r="D12" s="90"/>
       <c r="E12" s="52" t="s">
         <v>46</v>
       </c>
@@ -2395,8 +2427,8 @@
       <c r="A13" s="80">
         <v>0.5625</v>
       </c>
-      <c r="C13" s="90"/>
-      <c r="D13" s="87" t="s">
+      <c r="C13" s="91"/>
+      <c r="D13" s="88" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="52" t="s">
@@ -2411,11 +2443,11 @@
       <c r="A14" s="80">
         <v>0.58333333333333304</v>
       </c>
-      <c r="C14" s="90" t="s">
+      <c r="C14" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="88"/>
-      <c r="E14" s="87" t="s">
+      <c r="D14" s="90"/>
+      <c r="E14" s="88" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="85"/>
@@ -2427,11 +2459,11 @@
       <c r="A15" s="80">
         <v>0.60416666666666696</v>
       </c>
-      <c r="C15" s="90"/>
-      <c r="D15" s="87" t="s">
+      <c r="C15" s="91"/>
+      <c r="D15" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="88"/>
+      <c r="E15" s="90"/>
       <c r="F15" s="85"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -2441,11 +2473,11 @@
       <c r="A16" s="80">
         <v>0.625</v>
       </c>
-      <c r="C16" s="90" t="s">
+      <c r="C16" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="88"/>
-      <c r="E16" s="87" t="s">
+      <c r="D16" s="90"/>
+      <c r="E16" s="88" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="85"/>
@@ -2457,11 +2489,11 @@
       <c r="A17" s="80">
         <v>0.64583333333333404</v>
       </c>
-      <c r="C17" s="90"/>
-      <c r="D17" s="87" t="s">
+      <c r="C17" s="91"/>
+      <c r="D17" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="88"/>
+      <c r="E17" s="90"/>
       <c r="F17" s="85"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -2471,8 +2503,8 @@
       <c r="A18" s="80">
         <v>0.66666666666666696</v>
       </c>
-      <c r="C18" s="90"/>
-      <c r="D18" s="88"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="90"/>
       <c r="E18" s="51"/>
       <c r="F18" s="85"/>
       <c r="G18" s="3"/>
@@ -2502,7 +2534,7 @@
       <c r="C20" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="87" t="s">
+      <c r="D20" s="88" t="s">
         <v>29</v>
       </c>
       <c r="E20" s="51"/>
@@ -2515,10 +2547,10 @@
       <c r="A21" s="80">
         <v>0.72916666666666696</v>
       </c>
-      <c r="C21" s="90" t="s">
+      <c r="C21" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="88"/>
+      <c r="D21" s="90"/>
       <c r="E21" s="51"/>
       <c r="F21" s="85"/>
       <c r="G21" s="3"/>
@@ -2529,7 +2561,7 @@
       <c r="A22" s="80">
         <v>0.75</v>
       </c>
-      <c r="C22" s="90"/>
+      <c r="C22" s="91"/>
       <c r="D22" s="51" t="s">
         <v>37</v>
       </c>
@@ -2543,7 +2575,7 @@
       <c r="A23" s="80">
         <v>0.77083333333333404</v>
       </c>
-      <c r="C23" s="90"/>
+      <c r="C23" s="91"/>
       <c r="D23" s="51" t="s">
         <v>36</v>
       </c>
@@ -2626,21 +2658,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C9:C11"/>
     <mergeCell ref="E6:E9"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="D4:D6"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
wip: last commit of the week!
</commit_message>
<xml_diff>
--- a/__docs/diary.xlsx
+++ b/__docs/diary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9330"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="111">
   <si>
     <t>Felmerült problémák:</t>
   </si>
@@ -344,6 +344,21 @@
   </si>
   <si>
     <t>notebookban próbálom levezetni a pipline-t</t>
+  </si>
+  <si>
+    <t>binary fish</t>
+  </si>
+  <si>
+    <t>segmenting fish</t>
+  </si>
+  <si>
+    <t>binary image a pipelineból</t>
+  </si>
+  <si>
+    <t>SZEGMENTÁCIÓÓÓÓ</t>
+  </si>
+  <si>
+    <t>defekt</t>
   </si>
 </sst>
 </file>
@@ -1129,22 +1144,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -1427,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU22"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1627,7 +1642,9 @@
       <c r="N2" s="13">
         <v>0.36458333333333331</v>
       </c>
-      <c r="O2" s="13"/>
+      <c r="O2" s="13">
+        <v>0.40625</v>
+      </c>
       <c r="P2" s="52"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -1792,7 +1809,7 @@
       </c>
       <c r="O4" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.40625</v>
       </c>
       <c r="P4" s="52"/>
       <c r="Q4" s="55">
@@ -2327,19 +2344,19 @@
       <c r="P20" s="52"/>
     </row>
     <row r="21" spans="1:16" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="106">
+      <c r="B21" s="101">
         <f>HOUR(B4)</f>
         <v>8</v>
       </c>
-      <c r="C21" s="106">
+      <c r="C21" s="101">
         <f t="shared" ref="C21:E21" si="1">HOUR(C4)</f>
         <v>10</v>
       </c>
-      <c r="D21" s="106">
+      <c r="D21" s="101">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E21" s="106">
+      <c r="E21" s="101">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -2347,19 +2364,19 @@
         <f>SUM(B21:E21)</f>
         <v>37</v>
       </c>
-      <c r="G21" s="106">
+      <c r="G21" s="101">
         <f t="shared" ref="G21:J21" si="2">HOUR(G4)</f>
         <v>10</v>
       </c>
-      <c r="H21" s="106">
+      <c r="H21" s="101">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="I21" s="106">
+      <c r="I21" s="101">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="J21" s="106">
+      <c r="J21" s="101">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
@@ -2367,37 +2384,37 @@
         <f>SUM(G21:J21)</f>
         <v>38</v>
       </c>
-      <c r="L21" s="106">
+      <c r="L21" s="101">
         <f>HOUR(L4)</f>
         <v>10</v>
       </c>
-      <c r="M21" s="106">
+      <c r="M21" s="101">
         <f t="shared" ref="M21:O21" si="3">HOUR(M4)</f>
         <v>9</v>
       </c>
-      <c r="N21" s="106" t="e">
+      <c r="N21" s="101" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="O21" s="106">
+      <c r="O21" s="101" t="e">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="106">
+      <c r="B22" s="101">
         <f>MINUTE(B4)</f>
         <v>12</v>
       </c>
-      <c r="C22" s="106">
+      <c r="C22" s="101">
         <f t="shared" ref="C22:E22" si="4">MINUTE(C4)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="106">
+      <c r="D22" s="101">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="E22" s="106">
+      <c r="E22" s="101">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
@@ -2405,19 +2422,19 @@
         <f>SUM(B22:E22)</f>
         <v>40</v>
       </c>
-      <c r="G22" s="106">
+      <c r="G22" s="101">
         <f t="shared" ref="G22:J22" si="5">MINUTE(G4)</f>
         <v>41</v>
       </c>
-      <c r="H22" s="106">
+      <c r="H22" s="101">
         <f t="shared" si="5"/>
         <v>56</v>
       </c>
-      <c r="I22" s="106">
+      <c r="I22" s="101">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="J22" s="106">
+      <c r="J22" s="101">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
@@ -2425,21 +2442,21 @@
         <f>SUM(G22:J22)</f>
         <v>120</v>
       </c>
-      <c r="L22" s="106">
+      <c r="L22" s="101">
         <f>MINUTE(L4)</f>
         <v>12</v>
       </c>
-      <c r="M22" s="106">
+      <c r="M22" s="101">
         <f t="shared" ref="M22:O22" si="6">MINUTE(M4)</f>
         <v>30</v>
       </c>
-      <c r="N22" s="106" t="e">
+      <c r="N22" s="101" t="e">
         <f t="shared" si="6"/>
         <v>#NUM!</v>
       </c>
-      <c r="O22" s="106">
+      <c r="O22" s="101" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
@@ -2452,8 +2469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.28515625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2634,7 +2651,7 @@
       <c r="L2" s="98"/>
       <c r="M2" s="99"/>
       <c r="N2" s="99"/>
-      <c r="O2" s="96"/>
+      <c r="O2" s="99"/>
       <c r="P2" s="96"/>
       <c r="Q2" s="96"/>
       <c r="R2" s="96"/>
@@ -2662,7 +2679,7 @@
       <c r="L3" s="98"/>
       <c r="M3" s="99"/>
       <c r="N3" s="99"/>
-      <c r="O3" s="96"/>
+      <c r="O3" s="99"/>
       <c r="P3" s="96"/>
       <c r="Q3" s="96"/>
       <c r="R3" s="96"/>
@@ -2673,14 +2690,14 @@
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="93"/>
-      <c r="D4" s="102" t="s">
+      <c r="D4" s="103" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="71" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="82"/>
-      <c r="G4" s="102" t="s">
+      <c r="G4" s="103" t="s">
         <v>53</v>
       </c>
       <c r="H4" s="69" t="s">
@@ -2698,7 +2715,7 @@
       <c r="N4" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="96"/>
+      <c r="O4" s="99"/>
       <c r="P4" s="96"/>
       <c r="Q4" s="96"/>
       <c r="R4" s="96"/>
@@ -2709,32 +2726,34 @@
       </c>
       <c r="B5" s="71"/>
       <c r="C5" s="93"/>
-      <c r="D5" s="103"/>
+      <c r="D5" s="106"/>
       <c r="E5" s="71" t="s">
         <v>41</v>
       </c>
       <c r="F5" s="82"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="102" t="s">
+      <c r="G5" s="106"/>
+      <c r="H5" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="102" t="s">
+      <c r="I5" s="103" t="s">
         <v>28</v>
       </c>
       <c r="J5" s="72" t="s">
         <v>78</v>
       </c>
       <c r="K5" s="65"/>
-      <c r="L5" s="101" t="s">
+      <c r="L5" s="102" t="s">
         <v>74</v>
       </c>
       <c r="M5" s="96" t="s">
         <v>93</v>
       </c>
-      <c r="N5" s="101" t="s">
+      <c r="N5" s="102" t="s">
         <v>95</v>
       </c>
-      <c r="O5" s="96"/>
+      <c r="O5" s="96" t="s">
+        <v>28</v>
+      </c>
       <c r="P5" s="96"/>
       <c r="Q5" s="96"/>
       <c r="R5" s="96"/>
@@ -2748,23 +2767,25 @@
         <v>9</v>
       </c>
       <c r="D6" s="104"/>
-      <c r="E6" s="102" t="s">
+      <c r="E6" s="103" t="s">
         <v>46</v>
       </c>
       <c r="F6" s="82"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
+      <c r="G6" s="106"/>
+      <c r="H6" s="106"/>
       <c r="I6" s="104"/>
       <c r="J6" s="72" t="s">
         <v>79</v>
       </c>
       <c r="K6" s="65"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101" t="s">
+      <c r="L6" s="102"/>
+      <c r="M6" s="102" t="s">
         <v>96</v>
       </c>
-      <c r="N6" s="101"/>
-      <c r="O6" s="96"/>
+      <c r="N6" s="102"/>
+      <c r="O6" s="96" t="s">
+        <v>106</v>
+      </c>
       <c r="P6" s="96"/>
       <c r="Q6" s="96"/>
       <c r="R6" s="96"/>
@@ -2780,10 +2801,10 @@
       <c r="D7" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="103"/>
+      <c r="E7" s="106"/>
       <c r="F7" s="82"/>
-      <c r="G7" s="103"/>
-      <c r="H7" s="103"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="106"/>
       <c r="I7" s="72" t="s">
         <v>69</v>
       </c>
@@ -2791,10 +2812,12 @@
         <v>80</v>
       </c>
       <c r="K7" s="65"/>
-      <c r="L7" s="101"/>
-      <c r="M7" s="101"/>
-      <c r="N7" s="101"/>
-      <c r="O7" s="96"/>
+      <c r="L7" s="102"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="102"/>
+      <c r="O7" s="102" t="s">
+        <v>107</v>
+      </c>
       <c r="P7" s="96"/>
       <c r="Q7" s="96"/>
       <c r="R7" s="96"/>
@@ -2807,10 +2830,10 @@
       <c r="C8" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="102" t="s">
+      <c r="D8" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="103"/>
+      <c r="E8" s="106"/>
       <c r="F8" s="82"/>
       <c r="G8" s="104"/>
       <c r="H8" s="104"/>
@@ -2821,10 +2844,10 @@
         <v>81</v>
       </c>
       <c r="K8" s="65"/>
-      <c r="L8" s="101"/>
-      <c r="M8" s="101"/>
-      <c r="N8" s="101"/>
-      <c r="O8" s="96"/>
+      <c r="L8" s="102"/>
+      <c r="M8" s="102"/>
+      <c r="N8" s="102"/>
+      <c r="O8" s="102"/>
       <c r="P8" s="96"/>
       <c r="Q8" s="96"/>
       <c r="R8" s="96"/>
@@ -2837,26 +2860,26 @@
       <c r="C9" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="103"/>
+      <c r="D9" s="106"/>
       <c r="E9" s="104"/>
       <c r="F9" s="82"/>
       <c r="G9" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="102" t="s">
+      <c r="H9" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="102" t="s">
+      <c r="I9" s="103" t="s">
         <v>71</v>
       </c>
       <c r="J9" s="72" t="s">
         <v>73</v>
       </c>
       <c r="K9" s="65"/>
-      <c r="L9" s="101"/>
-      <c r="M9" s="101"/>
-      <c r="N9" s="101"/>
-      <c r="O9" s="96"/>
+      <c r="L9" s="102"/>
+      <c r="M9" s="102"/>
+      <c r="N9" s="102"/>
+      <c r="O9" s="102"/>
       <c r="P9" s="96"/>
       <c r="Q9" s="96"/>
       <c r="R9" s="96"/>
@@ -2867,24 +2890,26 @@
       </c>
       <c r="B10" s="71"/>
       <c r="C10" s="105"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="102" t="s">
+      <c r="D10" s="106"/>
+      <c r="E10" s="103" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="82"/>
-      <c r="G10" s="102" t="s">
+      <c r="G10" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="103"/>
-      <c r="I10" s="103"/>
-      <c r="J10" s="102" t="s">
+      <c r="H10" s="106"/>
+      <c r="I10" s="106"/>
+      <c r="J10" s="103" t="s">
         <v>82</v>
       </c>
       <c r="K10" s="65"/>
-      <c r="L10" s="101"/>
-      <c r="M10" s="101"/>
-      <c r="N10" s="101"/>
-      <c r="O10" s="96"/>
+      <c r="L10" s="102"/>
+      <c r="M10" s="102"/>
+      <c r="N10" s="102"/>
+      <c r="O10" s="96" t="s">
+        <v>15</v>
+      </c>
       <c r="P10" s="96"/>
       <c r="Q10" s="96"/>
       <c r="R10" s="96"/>
@@ -2895,22 +2920,24 @@
       </c>
       <c r="B11" s="71"/>
       <c r="C11" s="105"/>
-      <c r="D11" s="103"/>
+      <c r="D11" s="106"/>
       <c r="E11" s="104"/>
       <c r="F11" s="82"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
-      <c r="J11" s="103"/>
+      <c r="G11" s="106"/>
+      <c r="H11" s="106"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="106"/>
       <c r="K11" s="65"/>
-      <c r="L11" s="101"/>
+      <c r="L11" s="102"/>
       <c r="M11" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="N11" s="101" t="s">
+      <c r="N11" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="O11" s="96"/>
+      <c r="O11" s="102" t="s">
+        <v>109</v>
+      </c>
       <c r="P11" s="96"/>
       <c r="Q11" s="96"/>
       <c r="R11" s="96"/>
@@ -2929,18 +2956,18 @@
       </c>
       <c r="F12" s="82"/>
       <c r="G12" s="104"/>
-      <c r="H12" s="103"/>
-      <c r="I12" s="103"/>
+      <c r="H12" s="106"/>
+      <c r="I12" s="106"/>
       <c r="J12" s="104"/>
       <c r="K12" s="65"/>
-      <c r="L12" s="101" t="s">
+      <c r="L12" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="M12" s="101" t="s">
+      <c r="M12" s="102" t="s">
         <v>95</v>
       </c>
-      <c r="N12" s="101"/>
-      <c r="O12" s="96"/>
+      <c r="N12" s="102"/>
+      <c r="O12" s="102"/>
       <c r="P12" s="96"/>
       <c r="Q12" s="96"/>
       <c r="R12" s="96"/>
@@ -2951,7 +2978,7 @@
       </c>
       <c r="B13" s="71"/>
       <c r="C13" s="105"/>
-      <c r="D13" s="102" t="s">
+      <c r="D13" s="103" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="71" t="s">
@@ -2962,17 +2989,17 @@
         <v>56</v>
       </c>
       <c r="H13" s="104"/>
-      <c r="I13" s="103"/>
+      <c r="I13" s="106"/>
       <c r="J13" s="72" t="s">
         <v>84</v>
       </c>
       <c r="K13" s="65"/>
-      <c r="L13" s="101"/>
-      <c r="M13" s="101"/>
-      <c r="N13" s="101" t="s">
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="102" t="s">
         <v>105</v>
       </c>
-      <c r="O13" s="96"/>
+      <c r="O13" s="102"/>
       <c r="P13" s="96"/>
       <c r="Q13" s="96"/>
       <c r="R13" s="96"/>
@@ -2986,27 +3013,27 @@
         <v>16</v>
       </c>
       <c r="D14" s="104"/>
-      <c r="E14" s="102" t="s">
+      <c r="E14" s="103" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="82"/>
       <c r="G14" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="102" t="s">
+      <c r="H14" s="103" t="s">
         <v>15</v>
       </c>
       <c r="I14" s="104"/>
-      <c r="J14" s="102" t="s">
+      <c r="J14" s="103" t="s">
         <v>15</v>
       </c>
       <c r="K14" s="65"/>
-      <c r="L14" s="101" t="s">
+      <c r="L14" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="M14" s="101"/>
-      <c r="N14" s="101"/>
-      <c r="O14" s="96"/>
+      <c r="M14" s="102"/>
+      <c r="N14" s="102"/>
+      <c r="O14" s="102"/>
       <c r="P14" s="96"/>
       <c r="Q14" s="96"/>
       <c r="R14" s="96"/>
@@ -3017,24 +3044,24 @@
       </c>
       <c r="B15" s="71"/>
       <c r="C15" s="105"/>
-      <c r="D15" s="102" t="s">
+      <c r="D15" s="103" t="s">
         <v>29</v>
       </c>
       <c r="E15" s="104"/>
       <c r="F15" s="82"/>
-      <c r="G15" s="102" t="s">
+      <c r="G15" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="H15" s="103"/>
+      <c r="H15" s="106"/>
       <c r="I15" s="72" t="s">
         <v>21</v>
       </c>
       <c r="J15" s="104"/>
       <c r="K15" s="65"/>
-      <c r="L15" s="101"/>
-      <c r="M15" s="101"/>
-      <c r="N15" s="101"/>
-      <c r="O15" s="96"/>
+      <c r="L15" s="102"/>
+      <c r="M15" s="102"/>
+      <c r="N15" s="102"/>
+      <c r="O15" s="102"/>
       <c r="P15" s="96"/>
       <c r="Q15" s="96"/>
       <c r="R15" s="96"/>
@@ -3048,23 +3075,23 @@
         <v>18</v>
       </c>
       <c r="D16" s="104"/>
-      <c r="E16" s="102" t="s">
+      <c r="E16" s="103" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="82"/>
-      <c r="G16" s="103"/>
+      <c r="G16" s="106"/>
       <c r="H16" s="104"/>
-      <c r="I16" s="102" t="s">
+      <c r="I16" s="103" t="s">
         <v>72</v>
       </c>
       <c r="J16" s="72" t="s">
         <v>85</v>
       </c>
       <c r="K16" s="65"/>
-      <c r="L16" s="101"/>
-      <c r="M16" s="101"/>
-      <c r="N16" s="101"/>
-      <c r="O16" s="96"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="102"/>
+      <c r="N16" s="102"/>
+      <c r="O16" s="102"/>
       <c r="P16" s="96"/>
       <c r="Q16" s="96"/>
       <c r="R16" s="96"/>
@@ -3075,24 +3102,24 @@
       </c>
       <c r="B17" s="71"/>
       <c r="C17" s="105"/>
-      <c r="D17" s="102" t="s">
+      <c r="D17" s="103" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="104"/>
       <c r="F17" s="82"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="102" t="s">
+      <c r="G17" s="106"/>
+      <c r="H17" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="I17" s="103"/>
-      <c r="J17" s="102" t="s">
+      <c r="I17" s="106"/>
+      <c r="J17" s="103" t="s">
         <v>86</v>
       </c>
       <c r="K17" s="65"/>
-      <c r="L17" s="101"/>
-      <c r="M17" s="101"/>
-      <c r="N17" s="101"/>
-      <c r="O17" s="96"/>
+      <c r="L17" s="102"/>
+      <c r="M17" s="102"/>
+      <c r="N17" s="102"/>
+      <c r="O17" s="102"/>
       <c r="P17" s="96"/>
       <c r="Q17" s="96"/>
       <c r="R17" s="96"/>
@@ -3108,17 +3135,19 @@
         <v>21</v>
       </c>
       <c r="F18" s="82"/>
-      <c r="G18" s="103"/>
-      <c r="H18" s="103"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="106"/>
       <c r="I18" s="104"/>
-      <c r="J18" s="103"/>
+      <c r="J18" s="106"/>
       <c r="K18" s="65"/>
-      <c r="L18" s="101"/>
-      <c r="M18" s="101" t="s">
+      <c r="L18" s="102"/>
+      <c r="M18" s="102" t="s">
         <v>99</v>
       </c>
-      <c r="N18" s="101"/>
-      <c r="O18" s="96"/>
+      <c r="N18" s="102"/>
+      <c r="O18" s="102" t="s">
+        <v>110</v>
+      </c>
       <c r="P18" s="96"/>
       <c r="Q18" s="96"/>
       <c r="R18" s="96"/>
@@ -3134,23 +3163,23 @@
       <c r="D19" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="102" t="s">
+      <c r="E19" s="103" t="s">
         <v>48</v>
       </c>
       <c r="F19" s="82"/>
-      <c r="G19" s="103"/>
-      <c r="H19" s="103"/>
-      <c r="I19" s="102" t="s">
+      <c r="G19" s="106"/>
+      <c r="H19" s="106"/>
+      <c r="I19" s="103" t="s">
         <v>73</v>
       </c>
-      <c r="J19" s="103"/>
+      <c r="J19" s="106"/>
       <c r="K19" s="65"/>
-      <c r="L19" s="101"/>
-      <c r="M19" s="101"/>
+      <c r="L19" s="102"/>
+      <c r="M19" s="102"/>
       <c r="N19" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="96"/>
+      <c r="O19" s="102"/>
       <c r="P19" s="96"/>
       <c r="Q19" s="96"/>
       <c r="R19" s="96"/>
@@ -3163,24 +3192,24 @@
       <c r="C20" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="102" t="s">
+      <c r="D20" s="103" t="s">
         <v>29</v>
       </c>
       <c r="E20" s="104"/>
       <c r="F20" s="82"/>
-      <c r="G20" s="103"/>
-      <c r="H20" s="103"/>
+      <c r="G20" s="106"/>
+      <c r="H20" s="106"/>
       <c r="I20" s="104"/>
-      <c r="J20" s="103"/>
+      <c r="J20" s="106"/>
       <c r="K20" s="65"/>
       <c r="L20" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="M20" s="101" t="s">
+      <c r="M20" s="102" t="s">
         <v>95</v>
       </c>
       <c r="N20" s="96"/>
-      <c r="O20" s="96"/>
+      <c r="O20" s="102"/>
       <c r="P20" s="96"/>
       <c r="Q20" s="96"/>
       <c r="R20" s="96"/>
@@ -3198,17 +3227,17 @@
         <v>36</v>
       </c>
       <c r="F21" s="82"/>
-      <c r="G21" s="103"/>
+      <c r="G21" s="106"/>
       <c r="H21" s="104"/>
-      <c r="I21" s="102" t="s">
+      <c r="I21" s="103" t="s">
         <v>70</v>
       </c>
       <c r="J21" s="104"/>
       <c r="K21" s="65"/>
-      <c r="L21" s="101" t="s">
+      <c r="L21" s="102" t="s">
         <v>91</v>
       </c>
-      <c r="M21" s="101"/>
+      <c r="M21" s="102"/>
       <c r="N21" s="96"/>
       <c r="O21" s="96"/>
       <c r="P21" s="96"/>
@@ -3226,7 +3255,7 @@
       </c>
       <c r="E22" s="64"/>
       <c r="F22" s="82"/>
-      <c r="G22" s="103"/>
+      <c r="G22" s="106"/>
       <c r="H22" s="69" t="s">
         <v>21</v>
       </c>
@@ -3235,7 +3264,7 @@
         <v>87</v>
       </c>
       <c r="K22" s="65"/>
-      <c r="L22" s="101"/>
+      <c r="L22" s="102"/>
       <c r="M22" s="99"/>
       <c r="N22" s="96"/>
       <c r="O22" s="96"/>
@@ -3258,12 +3287,12 @@
       <c r="H23" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="I23" s="102" t="s">
+      <c r="I23" s="103" t="s">
         <v>74</v>
       </c>
       <c r="J23" s="64"/>
       <c r="K23" s="65"/>
-      <c r="L23" s="101"/>
+      <c r="L23" s="102"/>
       <c r="M23" s="99"/>
       <c r="N23" s="96"/>
       <c r="O23" s="96"/>
@@ -3291,8 +3320,8 @@
         <v>36</v>
       </c>
       <c r="M24" s="99"/>
-      <c r="N24" s="96"/>
-      <c r="O24" s="96"/>
+      <c r="N24" s="98"/>
+      <c r="O24" s="98"/>
       <c r="P24" s="96"/>
       <c r="Q24" s="96"/>
       <c r="R24" s="96"/>
@@ -3313,9 +3342,9 @@
       <c r="K25" s="65"/>
       <c r="L25" s="98"/>
       <c r="M25" s="99"/>
-      <c r="N25" s="96"/>
-      <c r="O25" s="96"/>
-      <c r="P25" s="96"/>
+      <c r="N25" s="98"/>
+      <c r="O25" s="98"/>
+      <c r="P25" s="98"/>
       <c r="Q25" s="96"/>
       <c r="R25" s="96"/>
     </row>
@@ -3335,9 +3364,9 @@
       <c r="K26" s="65"/>
       <c r="L26" s="98"/>
       <c r="M26" s="99"/>
-      <c r="N26" s="96"/>
-      <c r="O26" s="96"/>
-      <c r="P26" s="96"/>
+      <c r="N26" s="98"/>
+      <c r="O26" s="98"/>
+      <c r="P26" s="98"/>
       <c r="Q26" s="96"/>
       <c r="R26" s="96"/>
     </row>
@@ -3357,9 +3386,9 @@
       <c r="K27" s="65"/>
       <c r="L27" s="98"/>
       <c r="M27" s="99"/>
-      <c r="N27" s="96"/>
-      <c r="O27" s="96"/>
-      <c r="P27" s="96"/>
+      <c r="N27" s="98"/>
+      <c r="O27" s="98"/>
+      <c r="P27" s="98"/>
       <c r="Q27" s="96"/>
       <c r="R27" s="96"/>
     </row>
@@ -3378,8 +3407,8 @@
       <c r="J28" s="81"/>
       <c r="L28" s="98"/>
       <c r="M28" s="99"/>
-      <c r="N28" s="96"/>
-      <c r="O28" s="96"/>
+      <c r="N28" s="98"/>
+      <c r="O28" s="98"/>
       <c r="P28" s="96"/>
       <c r="Q28" s="96"/>
       <c r="R28" s="96"/>
@@ -3396,12 +3425,28 @@
       <c r="F31" s="76"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="N5:N10"/>
-    <mergeCell ref="N13:N18"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="C16:C18"/>
+  <mergeCells count="46">
+    <mergeCell ref="O7:O9"/>
+    <mergeCell ref="O11:O17"/>
+    <mergeCell ref="O18:O20"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="M6:M10"/>
+    <mergeCell ref="M12:M17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="L14:L19"/>
+    <mergeCell ref="L21:L23"/>
+    <mergeCell ref="L5:L11"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="H17:H21"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="I21:I22"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C15"/>
@@ -3417,29 +3462,16 @@
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="H9:H13"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="N5:N10"/>
+    <mergeCell ref="N13:N18"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="C16:C18"/>
     <mergeCell ref="I9:I14"/>
     <mergeCell ref="I16:I18"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="H17:H21"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
     <mergeCell ref="J10:J12"/>
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="J17:J21"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="M6:M10"/>
-    <mergeCell ref="M12:M17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="L14:L19"/>
-    <mergeCell ref="L21:L23"/>
-    <mergeCell ref="L5:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3451,7 +3483,7 @@
   <dimension ref="A1:AH26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="105.7109375" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3902,8 +3934,10 @@
       <c r="AH12" s="75"/>
     </row>
     <row r="13" spans="1:34" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="74"/>
-      <c r="B13" s="76"/>
+      <c r="A13" s="61">
+        <v>44770</v>
+      </c>
+      <c r="B13" s="80"/>
       <c r="C13" s="76"/>
       <c r="D13" s="76"/>
       <c r="E13" s="76"/>
@@ -3939,7 +3973,9 @@
     </row>
     <row r="14" spans="1:34" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="74"/>
-      <c r="B14" s="76"/>
+      <c r="B14" s="76" t="s">
+        <v>108</v>
+      </c>
       <c r="C14" s="76"/>
       <c r="D14" s="76"/>
       <c r="E14" s="76"/>

</xml_diff>

<commit_message>
feat: fish labeling and mask (notebook)
</commit_message>
<xml_diff>
--- a/__docs/diary.xlsx
+++ b/__docs/diary.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="118">
   <si>
     <t>Felmerült problémák:</t>
   </si>
@@ -359,6 +359,27 @@
   </si>
   <si>
     <t>defekt</t>
+  </si>
+  <si>
+    <t>4th week</t>
+  </si>
+  <si>
+    <t>a fish szegmentálással ment a múlthét, de még nem működik</t>
+  </si>
+  <si>
+    <t>a jupyter elindításánál valamiért nem találja sosem a terminal_msg modult</t>
+  </si>
+  <si>
+    <t>írni MSc iránt</t>
+  </si>
+  <si>
+    <t>érdeklődni szakdoga iránt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">születésnapok </t>
+  </si>
+  <si>
+    <t>elpakolás és commit</t>
   </si>
 </sst>
 </file>
@@ -1442,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1646,7 +1667,9 @@
         <v>0.40625</v>
       </c>
       <c r="P2" s="52"/>
-      <c r="Q2" s="4"/>
+      <c r="Q2" s="4">
+        <v>0.37291666666666662</v>
+      </c>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
@@ -1721,7 +1744,9 @@
       <c r="N3" s="16"/>
       <c r="O3" s="16"/>
       <c r="P3" s="52"/>
-      <c r="Q3" s="7"/>
+      <c r="Q3" s="7">
+        <v>0.76736111111111116</v>
+      </c>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
@@ -1814,7 +1839,7 @@
       <c r="P4" s="52"/>
       <c r="Q4" s="55">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.39444444444444454</v>
       </c>
       <c r="R4" s="55">
         <f t="shared" si="0"/>
@@ -1964,6 +1989,9 @@
       </c>
       <c r="O5" s="19"/>
       <c r="P5" s="52"/>
+      <c r="Q5" s="10" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="6" spans="1:47" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
@@ -2092,6 +2120,9 @@
       </c>
       <c r="O10" s="33"/>
       <c r="P10" s="52"/>
+      <c r="Q10" s="34" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="11" spans="1:47" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
@@ -2467,10 +2498,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU31"/>
+  <dimension ref="A1:AS31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.28515625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2489,11 +2520,14 @@
     <col min="12" max="12" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="38.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="41.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="47" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="16384" width="32.28515625" style="1"/>
+    <col min="15" max="15" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="45" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="16384" width="32.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="60" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" s="60" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="63"/>
       <c r="B1" s="61">
         <v>44753</v>
@@ -2537,104 +2571,98 @@
       <c r="O1" s="60">
         <v>44770</v>
       </c>
-      <c r="P1" s="60">
-        <v>44771</v>
-      </c>
-      <c r="Q1" s="60">
-        <v>44772</v>
-      </c>
-      <c r="R1" s="60">
-        <v>44773</v>
-      </c>
-      <c r="S1" s="60">
+      <c r="P1" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q1" s="67">
         <v>44774</v>
       </c>
-      <c r="T1" s="60">
+      <c r="R1" s="67">
         <v>44775</v>
       </c>
-      <c r="U1" s="60">
+      <c r="S1" s="67">
         <v>44776</v>
       </c>
-      <c r="V1" s="60">
+      <c r="T1" s="67">
         <v>44777</v>
       </c>
-      <c r="W1" s="60">
+      <c r="U1" s="67">
         <v>44778</v>
       </c>
-      <c r="X1" s="60">
+      <c r="V1" s="67">
         <v>44779</v>
       </c>
-      <c r="Y1" s="60">
+      <c r="W1" s="67">
         <v>44780</v>
       </c>
-      <c r="Z1" s="60">
+      <c r="X1" s="67">
         <v>44781</v>
       </c>
-      <c r="AA1" s="60">
+      <c r="Y1" s="67">
         <v>44782</v>
       </c>
-      <c r="AB1" s="60">
+      <c r="Z1" s="67">
         <v>44783</v>
       </c>
-      <c r="AC1" s="60">
+      <c r="AA1" s="67">
         <v>44784</v>
       </c>
-      <c r="AD1" s="60">
+      <c r="AB1" s="67">
         <v>44785</v>
       </c>
-      <c r="AE1" s="60">
+      <c r="AC1" s="67">
         <v>44786</v>
       </c>
-      <c r="AF1" s="60">
+      <c r="AD1" s="67">
         <v>44787</v>
       </c>
+      <c r="AE1" s="67">
+        <v>44788</v>
+      </c>
+      <c r="AF1" s="67">
+        <v>44789</v>
+      </c>
       <c r="AG1" s="60">
-        <v>44788</v>
+        <v>44790</v>
       </c>
       <c r="AH1" s="60">
-        <v>44789</v>
+        <v>44791</v>
       </c>
       <c r="AI1" s="60">
-        <v>44790</v>
+        <v>44792</v>
       </c>
       <c r="AJ1" s="60">
-        <v>44791</v>
+        <v>44793</v>
       </c>
       <c r="AK1" s="60">
-        <v>44792</v>
+        <v>44794</v>
       </c>
       <c r="AL1" s="60">
-        <v>44793</v>
+        <v>44795</v>
       </c>
       <c r="AM1" s="60">
-        <v>44794</v>
+        <v>44796</v>
       </c>
       <c r="AN1" s="60">
-        <v>44795</v>
+        <v>44797</v>
       </c>
       <c r="AO1" s="60">
-        <v>44796</v>
+        <v>44798</v>
       </c>
       <c r="AP1" s="60">
-        <v>44797</v>
+        <v>44799</v>
       </c>
       <c r="AQ1" s="60">
-        <v>44798</v>
+        <v>44800</v>
       </c>
       <c r="AR1" s="60">
-        <v>44799</v>
+        <v>44801</v>
       </c>
       <c r="AS1" s="60">
-        <v>44800</v>
-      </c>
-      <c r="AT1" s="60">
-        <v>44801</v>
-      </c>
-      <c r="AU1" s="60">
         <v>44802</v>
       </c>
     </row>
-    <row r="2" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="91">
         <v>0.33333333333333331</v>
       </c>
@@ -2652,11 +2680,10 @@
       <c r="M2" s="99"/>
       <c r="N2" s="99"/>
       <c r="O2" s="99"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-    </row>
-    <row r="3" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="99"/>
+      <c r="Q2" s="99"/>
+    </row>
+    <row r="3" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="91">
         <v>0.35416666666666669</v>
       </c>
@@ -2680,11 +2707,10 @@
       <c r="M3" s="99"/>
       <c r="N3" s="99"/>
       <c r="O3" s="99"/>
-      <c r="P3" s="96"/>
-      <c r="Q3" s="96"/>
-      <c r="R3" s="96"/>
-    </row>
-    <row r="4" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P3" s="99"/>
+      <c r="Q3" s="99"/>
+    </row>
+    <row r="4" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="91">
         <v>0.375</v>
       </c>
@@ -2716,11 +2742,12 @@
         <v>28</v>
       </c>
       <c r="O4" s="99"/>
-      <c r="P4" s="96"/>
-      <c r="Q4" s="96"/>
-      <c r="R4" s="96"/>
-    </row>
-    <row r="5" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="99"/>
+      <c r="Q4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="91">
         <v>0.39583333333333298</v>
       </c>
@@ -2754,11 +2781,9 @@
       <c r="O5" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="96"/>
-      <c r="Q5" s="96"/>
-      <c r="R5" s="96"/>
-    </row>
-    <row r="6" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P5" s="99"/>
+    </row>
+    <row r="6" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="91">
         <v>0.41666666666666702</v>
       </c>
@@ -2786,11 +2811,9 @@
       <c r="O6" s="96" t="s">
         <v>106</v>
       </c>
-      <c r="P6" s="96"/>
-      <c r="Q6" s="96"/>
-      <c r="R6" s="96"/>
-    </row>
-    <row r="7" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P6" s="99"/>
+    </row>
+    <row r="7" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="91">
         <v>0.4375</v>
       </c>
@@ -2818,11 +2841,9 @@
       <c r="O7" s="102" t="s">
         <v>107</v>
       </c>
-      <c r="P7" s="96"/>
-      <c r="Q7" s="96"/>
-      <c r="R7" s="96"/>
-    </row>
-    <row r="8" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P7" s="99"/>
+    </row>
+    <row r="8" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="91">
         <v>0.45833333333333298</v>
       </c>
@@ -2848,11 +2869,9 @@
       <c r="M8" s="102"/>
       <c r="N8" s="102"/>
       <c r="O8" s="102"/>
-      <c r="P8" s="96"/>
-      <c r="Q8" s="96"/>
-      <c r="R8" s="96"/>
-    </row>
-    <row r="9" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P8" s="99"/>
+    </row>
+    <row r="9" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="91">
         <v>0.47916666666666702</v>
       </c>
@@ -2880,11 +2899,9 @@
       <c r="M9" s="102"/>
       <c r="N9" s="102"/>
       <c r="O9" s="102"/>
-      <c r="P9" s="96"/>
-      <c r="Q9" s="96"/>
-      <c r="R9" s="96"/>
-    </row>
-    <row r="10" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P9" s="99"/>
+    </row>
+    <row r="10" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="91">
         <v>0.5</v>
       </c>
@@ -2910,11 +2927,12 @@
       <c r="O10" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="P10" s="96"/>
-      <c r="Q10" s="96"/>
-      <c r="R10" s="96"/>
-    </row>
-    <row r="11" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P10" s="99"/>
+      <c r="Q10" s="102" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="91">
         <v>0.52083333333333304</v>
       </c>
@@ -2938,11 +2956,10 @@
       <c r="O11" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="P11" s="96"/>
-      <c r="Q11" s="96"/>
-      <c r="R11" s="96"/>
-    </row>
-    <row r="12" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="99"/>
+      <c r="Q11" s="102"/>
+    </row>
+    <row r="12" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="91">
         <v>0.54166666666666696</v>
       </c>
@@ -2968,11 +2985,9 @@
       </c>
       <c r="N12" s="102"/>
       <c r="O12" s="102"/>
-      <c r="P12" s="96"/>
-      <c r="Q12" s="96"/>
-      <c r="R12" s="96"/>
-    </row>
-    <row r="13" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="99"/>
+    </row>
+    <row r="13" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="91">
         <v>0.5625</v>
       </c>
@@ -3000,11 +3015,9 @@
         <v>105</v>
       </c>
       <c r="O13" s="102"/>
-      <c r="P13" s="96"/>
-      <c r="Q13" s="96"/>
-      <c r="R13" s="96"/>
-    </row>
-    <row r="14" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="99"/>
+    </row>
+    <row r="14" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="91">
         <v>0.58333333333333304</v>
       </c>
@@ -3034,11 +3047,9 @@
       <c r="M14" s="102"/>
       <c r="N14" s="102"/>
       <c r="O14" s="102"/>
-      <c r="P14" s="96"/>
-      <c r="Q14" s="96"/>
-      <c r="R14" s="96"/>
-    </row>
-    <row r="15" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P14" s="99"/>
+    </row>
+    <row r="15" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="91">
         <v>0.60416666666666696</v>
       </c>
@@ -3062,11 +3073,9 @@
       <c r="M15" s="102"/>
       <c r="N15" s="102"/>
       <c r="O15" s="102"/>
-      <c r="P15" s="96"/>
-      <c r="Q15" s="96"/>
-      <c r="R15" s="96"/>
-    </row>
-    <row r="16" spans="1:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P15" s="99"/>
+    </row>
+    <row r="16" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="91">
         <v>0.625</v>
       </c>
@@ -3092,11 +3101,9 @@
       <c r="M16" s="102"/>
       <c r="N16" s="102"/>
       <c r="O16" s="102"/>
-      <c r="P16" s="96"/>
-      <c r="Q16" s="96"/>
-      <c r="R16" s="96"/>
-    </row>
-    <row r="17" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P16" s="99"/>
+    </row>
+    <row r="17" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="91">
         <v>0.64583333333333404</v>
       </c>
@@ -3120,11 +3127,9 @@
       <c r="M17" s="102"/>
       <c r="N17" s="102"/>
       <c r="O17" s="102"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="96"/>
-    </row>
-    <row r="18" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P17" s="99"/>
+    </row>
+    <row r="18" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="91">
         <v>0.66666666666666696</v>
       </c>
@@ -3148,11 +3153,9 @@
       <c r="O18" s="102" t="s">
         <v>110</v>
       </c>
-      <c r="P18" s="96"/>
-      <c r="Q18" s="96"/>
-      <c r="R18" s="96"/>
-    </row>
-    <row r="19" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P18" s="99"/>
+    </row>
+    <row r="19" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="91">
         <v>0.6875</v>
       </c>
@@ -3180,11 +3183,9 @@
         <v>21</v>
       </c>
       <c r="O19" s="102"/>
-      <c r="P19" s="96"/>
-      <c r="Q19" s="96"/>
-      <c r="R19" s="96"/>
-    </row>
-    <row r="20" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P19" s="99"/>
+    </row>
+    <row r="20" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="91">
         <v>0.70833333333333404</v>
       </c>
@@ -3210,11 +3211,9 @@
       </c>
       <c r="N20" s="96"/>
       <c r="O20" s="102"/>
-      <c r="P20" s="96"/>
-      <c r="Q20" s="96"/>
-      <c r="R20" s="96"/>
-    </row>
-    <row r="21" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P20" s="99"/>
+    </row>
+    <row r="21" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="91">
         <v>0.72916666666666696</v>
       </c>
@@ -3240,11 +3239,9 @@
       <c r="M21" s="102"/>
       <c r="N21" s="96"/>
       <c r="O21" s="96"/>
-      <c r="P21" s="96"/>
-      <c r="Q21" s="96"/>
-      <c r="R21" s="96"/>
-    </row>
-    <row r="22" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P21" s="99"/>
+    </row>
+    <row r="22" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="91">
         <v>0.75</v>
       </c>
@@ -3268,11 +3265,12 @@
       <c r="M22" s="99"/>
       <c r="N22" s="96"/>
       <c r="O22" s="96"/>
-      <c r="P22" s="96"/>
-      <c r="Q22" s="96"/>
-      <c r="R22" s="96"/>
-    </row>
-    <row r="23" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P22" s="99"/>
+      <c r="Q22" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="91">
         <v>0.77083333333333404</v>
       </c>
@@ -3296,11 +3294,10 @@
       <c r="M23" s="99"/>
       <c r="N23" s="96"/>
       <c r="O23" s="96"/>
-      <c r="P23" s="96"/>
-      <c r="Q23" s="96"/>
-      <c r="R23" s="96"/>
-    </row>
-    <row r="24" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P23" s="99"/>
+      <c r="Q23" s="98"/>
+    </row>
+    <row r="24" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="91">
         <v>0.79166666666666696</v>
       </c>
@@ -3322,11 +3319,10 @@
       <c r="M24" s="99"/>
       <c r="N24" s="98"/>
       <c r="O24" s="98"/>
-      <c r="P24" s="96"/>
-      <c r="Q24" s="96"/>
-      <c r="R24" s="96"/>
-    </row>
-    <row r="25" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P24" s="98"/>
+      <c r="Q24" s="98"/>
+    </row>
+    <row r="25" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="91">
         <v>0.8125</v>
       </c>
@@ -3345,10 +3341,9 @@
       <c r="N25" s="98"/>
       <c r="O25" s="98"/>
       <c r="P25" s="98"/>
-      <c r="Q25" s="96"/>
-      <c r="R25" s="96"/>
-    </row>
-    <row r="26" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q25" s="98"/>
+    </row>
+    <row r="26" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="91">
         <v>0.83333333333333304</v>
       </c>
@@ -3367,10 +3362,9 @@
       <c r="N26" s="98"/>
       <c r="O26" s="98"/>
       <c r="P26" s="98"/>
-      <c r="Q26" s="96"/>
-      <c r="R26" s="96"/>
-    </row>
-    <row r="27" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q26" s="98"/>
+    </row>
+    <row r="27" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="91">
         <v>0.85416666666666596</v>
       </c>
@@ -3389,10 +3383,9 @@
       <c r="N27" s="98"/>
       <c r="O27" s="98"/>
       <c r="P27" s="98"/>
-      <c r="Q27" s="96"/>
-      <c r="R27" s="96"/>
-    </row>
-    <row r="28" spans="1:18" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q27" s="98"/>
+    </row>
+    <row r="28" spans="1:17" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="91">
         <v>0.874999999999999</v>
       </c>
@@ -3409,23 +3402,23 @@
       <c r="M28" s="99"/>
       <c r="N28" s="98"/>
       <c r="O28" s="98"/>
-      <c r="P28" s="96"/>
-      <c r="Q28" s="96"/>
-      <c r="R28" s="96"/>
-    </row>
-    <row r="29" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P28" s="98"/>
+      <c r="Q28" s="98"/>
+    </row>
+    <row r="29" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="89"/>
       <c r="E29" s="89"/>
       <c r="F29" s="76"/>
     </row>
-    <row r="30" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F30" s="76"/>
     </row>
-    <row r="31" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F31" s="76"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="47">
+    <mergeCell ref="Q10:Q11"/>
     <mergeCell ref="O7:O9"/>
     <mergeCell ref="O11:O17"/>
     <mergeCell ref="O18:O20"/>
@@ -3439,6 +3432,10 @@
     <mergeCell ref="L21:L23"/>
     <mergeCell ref="L5:L11"/>
     <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="N5:N10"/>
+    <mergeCell ref="H9:H13"/>
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="H17:H21"/>
     <mergeCell ref="D4:D6"/>
@@ -3446,7 +3443,20 @@
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="D17:D18"/>
-    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="G15:G23"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="N13:N18"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="I9:I14"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="J17:J21"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C15"/>
@@ -3455,23 +3465,6 @@
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="G4:G8"/>
     <mergeCell ref="G10:G12"/>
-    <mergeCell ref="G15:G23"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="H9:H13"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="N5:N10"/>
-    <mergeCell ref="N13:N18"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="I9:I14"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="J17:J21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3483,7 +3476,7 @@
   <dimension ref="A1:AH26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="105.7109375" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4082,8 +4075,10 @@
       <c r="AH16" s="75"/>
     </row>
     <row r="17" spans="1:34" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="74"/>
-      <c r="B17" s="76"/>
+      <c r="A17" s="61">
+        <v>44770</v>
+      </c>
+      <c r="B17" s="80"/>
       <c r="C17" s="76"/>
       <c r="D17" s="76"/>
       <c r="E17" s="79"/>
@@ -4119,7 +4114,9 @@
     </row>
     <row r="18" spans="1:34" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="74"/>
-      <c r="B18" s="76"/>
+      <c r="B18" s="76" t="s">
+        <v>114</v>
+      </c>
       <c r="C18" s="79"/>
       <c r="D18" s="79"/>
       <c r="E18" s="76"/>
@@ -4154,7 +4151,9 @@
       <c r="AH18" s="75"/>
     </row>
     <row r="19" spans="1:34" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="76"/>
+      <c r="B19" s="76" t="s">
+        <v>115</v>
+      </c>
       <c r="C19" s="79"/>
       <c r="D19" s="76"/>
       <c r="E19" s="76"/>
@@ -4189,7 +4188,9 @@
       <c r="AH19" s="75"/>
     </row>
     <row r="20" spans="1:34" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="76"/>
+      <c r="B20" s="76" t="s">
+        <v>116</v>
+      </c>
       <c r="C20" s="76"/>
       <c r="D20" s="76"/>
       <c r="E20" s="79"/>

</xml_diff>

<commit_message>
feat: pipeline from notebook WIP!
</commit_message>
<xml_diff>
--- a/__docs/diary.xlsx
+++ b/__docs/diary.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="126">
   <si>
     <t>Felmerült problémák:</t>
   </si>
@@ -389,6 +389,21 @@
   </si>
   <si>
     <t>yen thresholding ot éppen implementálom a notebook ból</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>szabi</t>
+  </si>
+  <si>
+    <t>a wiener filtert nem használtam, nem tudom MATLABBAN hogyan néz ki</t>
+  </si>
+  <si>
+    <t>yen_th</t>
+  </si>
+  <si>
+    <t>5th week</t>
   </si>
 </sst>
 </file>
@@ -398,7 +413,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,6 +505,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="72"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -906,7 +929,7 @@
     <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1208,6 +1231,18 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="135"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="135"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1508,8 +1543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="P10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1526,7 +1561,12 @@
     <col min="11" max="11" width="19.85546875" style="2" customWidth="1"/>
     <col min="13" max="13" width="63.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.85546875" style="100" bestFit="1" customWidth="1"/>
-    <col min="21" max="26" width="55" style="100"/>
+    <col min="17" max="17" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="66.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="2.42578125" style="100" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.5703125" style="100" customWidth="1"/>
+    <col min="24" max="26" width="55" style="100"/>
     <col min="35" max="37" width="55" style="2"/>
   </cols>
   <sheetData>
@@ -1584,16 +1624,14 @@
       <c r="S1" s="43">
         <v>44776</v>
       </c>
-      <c r="T1" s="43">
+      <c r="T1" s="104">
         <v>44777</v>
       </c>
-      <c r="U1" s="43">
-        <v>44778</v>
-      </c>
-      <c r="V1" s="43">
-        <v>44779</v>
-      </c>
-      <c r="W1" s="43">
+      <c r="U1" s="52"/>
+      <c r="V1" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="W1" s="104">
         <v>44780</v>
       </c>
       <c r="X1" s="43">
@@ -1706,33 +1744,37 @@
         <v>0.36874999999999997</v>
       </c>
       <c r="N2" s="13">
-        <v>0.36458333333333331</v>
+        <v>0.36527777777777781</v>
       </c>
       <c r="O2" s="13">
-        <v>0.40625</v>
+        <v>0.40486111111111112</v>
       </c>
       <c r="P2" s="52"/>
-      <c r="Q2" s="4">
+      <c r="Q2" s="13">
         <v>0.37291666666666662</v>
       </c>
-      <c r="R2" s="4">
-        <v>0.4145833333333333</v>
-      </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
+      <c r="R2" s="13">
+        <v>0.41388888888888892</v>
+      </c>
+      <c r="S2" s="13">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="T2" s="106" t="s">
+        <v>122</v>
+      </c>
+      <c r="U2" s="106"/>
+      <c r="V2" s="106"/>
+      <c r="W2" s="106"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
       <c r="AH2" s="4"/>
       <c r="AI2" s="5"/>
       <c r="AJ2" s="5"/>
@@ -1788,31 +1830,37 @@
       <c r="M3" s="17">
         <v>0.76458333333333339</v>
       </c>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
+      <c r="N3" s="16">
+        <v>0.83888888888888891</v>
+      </c>
+      <c r="O3" s="16">
+        <v>0.78263888888888899</v>
+      </c>
       <c r="P3" s="52"/>
-      <c r="Q3" s="7">
-        <v>0.76736111111111116</v>
-      </c>
-      <c r="R3" s="7">
-        <v>0.76041666666666663</v>
-      </c>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
-      <c r="AD3" s="7"/>
-      <c r="AE3" s="7"/>
-      <c r="AF3" s="7"/>
-      <c r="AG3" s="7"/>
-      <c r="AH3" s="7"/>
+      <c r="Q3" s="16">
+        <v>0.7729166666666667</v>
+      </c>
+      <c r="R3" s="16">
+        <v>0.7715277777777777</v>
+      </c>
+      <c r="S3" s="16">
+        <v>0.64027777777777783</v>
+      </c>
+      <c r="T3" s="106"/>
+      <c r="U3" s="106"/>
+      <c r="V3" s="106"/>
+      <c r="W3" s="106"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="16"/>
+      <c r="AD3" s="16"/>
+      <c r="AE3" s="16"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="16"/>
+      <c r="AH3" s="16"/>
       <c r="AI3" s="8"/>
       <c r="AJ3" s="8"/>
       <c r="AK3" s="8"/>
@@ -1879,78 +1927,66 @@
       </c>
       <c r="N4" s="55">
         <f>N3-N2</f>
-        <v>-0.36458333333333331</v>
+        <v>0.47361111111111109</v>
       </c>
       <c r="O4" s="55">
         <f t="shared" si="0"/>
-        <v>-0.40625</v>
+        <v>0.37777777777777788</v>
       </c>
       <c r="P4" s="52"/>
-      <c r="Q4" s="55">
+      <c r="Q4" s="105">
         <f t="shared" si="0"/>
-        <v>0.39444444444444454</v>
-      </c>
-      <c r="R4" s="55">
+        <v>0.40000000000000008</v>
+      </c>
+      <c r="R4" s="105">
         <f t="shared" si="0"/>
-        <v>0.34583333333333333</v>
-      </c>
-      <c r="S4" s="55">
+        <v>0.35763888888888878</v>
+      </c>
+      <c r="S4" s="105">
+        <f t="shared" si="0"/>
+        <v>0.24444444444444452</v>
+      </c>
+      <c r="T4" s="106"/>
+      <c r="U4" s="106"/>
+      <c r="V4" s="106"/>
+      <c r="W4" s="106"/>
+      <c r="X4" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T4" s="55">
+      <c r="Y4" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U4" s="55">
+      <c r="Z4" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V4" s="55">
+      <c r="AA4" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W4" s="55">
+      <c r="AB4" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X4" s="55">
+      <c r="AC4" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Y4" s="55">
+      <c r="AD4" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Z4" s="55">
+      <c r="AE4" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA4" s="55">
+      <c r="AF4" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB4" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AC4" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD4" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AE4" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AF4" s="55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AG4" s="55">
+      <c r="AG4" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2038,9 +2074,27 @@
       </c>
       <c r="O5" s="19"/>
       <c r="P5" s="52"/>
-      <c r="Q5" s="10" t="s">
+      <c r="Q5" s="19" t="s">
         <v>112</v>
       </c>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="T5" s="106"/>
+      <c r="U5" s="106"/>
+      <c r="V5" s="106"/>
+      <c r="W5" s="106"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="19"/>
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="19"/>
+      <c r="AG5" s="19"/>
     </row>
     <row r="6" spans="1:47" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
@@ -2069,6 +2123,23 @@
       <c r="N6" s="19"/>
       <c r="O6" s="19"/>
       <c r="P6" s="52"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="106"/>
+      <c r="U6" s="106"/>
+      <c r="V6" s="106"/>
+      <c r="W6" s="106"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="19"/>
+      <c r="AF6" s="19"/>
+      <c r="AG6" s="19"/>
     </row>
     <row r="7" spans="1:47" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
@@ -2089,6 +2160,23 @@
       <c r="N7" s="19"/>
       <c r="O7" s="19"/>
       <c r="P7" s="52"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="106"/>
+      <c r="U7" s="106"/>
+      <c r="V7" s="106"/>
+      <c r="W7" s="106"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="19"/>
+      <c r="AC7" s="19"/>
+      <c r="AD7" s="19"/>
+      <c r="AE7" s="19"/>
+      <c r="AF7" s="19"/>
+      <c r="AG7" s="19"/>
     </row>
     <row r="8" spans="1:47" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -2109,6 +2197,23 @@
       <c r="N8" s="19"/>
       <c r="O8" s="19"/>
       <c r="P8" s="52"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="106"/>
+      <c r="U8" s="106"/>
+      <c r="V8" s="106"/>
+      <c r="W8" s="106"/>
+      <c r="X8" s="19"/>
+      <c r="Y8" s="19"/>
+      <c r="Z8" s="19"/>
+      <c r="AA8" s="19"/>
+      <c r="AB8" s="19"/>
+      <c r="AC8" s="19"/>
+      <c r="AD8" s="19"/>
+      <c r="AE8" s="19"/>
+      <c r="AF8" s="19"/>
+      <c r="AG8" s="19"/>
     </row>
     <row r="9" spans="1:47" s="31" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28"/>
@@ -2127,6 +2232,23 @@
       <c r="N9" s="30"/>
       <c r="O9" s="30"/>
       <c r="P9" s="52"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="106"/>
+      <c r="U9" s="106"/>
+      <c r="V9" s="106"/>
+      <c r="W9" s="106"/>
+      <c r="X9" s="30"/>
+      <c r="Y9" s="30"/>
+      <c r="Z9" s="30"/>
+      <c r="AA9" s="30"/>
+      <c r="AB9" s="30"/>
+      <c r="AC9" s="30"/>
+      <c r="AD9" s="30"/>
+      <c r="AE9" s="30"/>
+      <c r="AF9" s="30"/>
+      <c r="AG9" s="30"/>
     </row>
     <row r="10" spans="1:47" s="34" customFormat="1" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
@@ -2169,12 +2291,27 @@
       </c>
       <c r="O10" s="33"/>
       <c r="P10" s="52"/>
-      <c r="Q10" s="34" t="s">
+      <c r="Q10" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="S10" s="34" t="s">
-        <v>120</v>
-      </c>
+      <c r="R10" s="33"/>
+      <c r="S10" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="T10" s="106"/>
+      <c r="U10" s="106"/>
+      <c r="V10" s="106"/>
+      <c r="W10" s="106"/>
+      <c r="X10" s="33"/>
+      <c r="Y10" s="33"/>
+      <c r="Z10" s="33"/>
+      <c r="AA10" s="33"/>
+      <c r="AB10" s="33"/>
+      <c r="AC10" s="33"/>
+      <c r="AD10" s="33"/>
+      <c r="AE10" s="33"/>
+      <c r="AF10" s="33"/>
+      <c r="AG10" s="33"/>
     </row>
     <row r="11" spans="1:47" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
@@ -2211,6 +2348,23 @@
       <c r="N11" s="22"/>
       <c r="O11" s="22"/>
       <c r="P11" s="52"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="106"/>
+      <c r="U11" s="106"/>
+      <c r="V11" s="106"/>
+      <c r="W11" s="106"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="22"/>
+      <c r="Z11" s="22"/>
+      <c r="AA11" s="22"/>
+      <c r="AB11" s="22"/>
+      <c r="AC11" s="22"/>
+      <c r="AD11" s="22"/>
+      <c r="AE11" s="22"/>
+      <c r="AF11" s="22"/>
+      <c r="AG11" s="22"/>
     </row>
     <row r="12" spans="1:47" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
@@ -2241,6 +2395,23 @@
       </c>
       <c r="O12" s="22"/>
       <c r="P12" s="52"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="106"/>
+      <c r="U12" s="106"/>
+      <c r="V12" s="106"/>
+      <c r="W12" s="106"/>
+      <c r="X12" s="22"/>
+      <c r="Y12" s="22"/>
+      <c r="Z12" s="22"/>
+      <c r="AA12" s="22"/>
+      <c r="AB12" s="22"/>
+      <c r="AC12" s="22"/>
+      <c r="AD12" s="22"/>
+      <c r="AE12" s="22"/>
+      <c r="AF12" s="22"/>
+      <c r="AG12" s="22"/>
     </row>
     <row r="13" spans="1:47" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
@@ -2263,6 +2434,23 @@
       <c r="N13" s="22"/>
       <c r="O13" s="22"/>
       <c r="P13" s="52"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="106"/>
+      <c r="U13" s="106"/>
+      <c r="V13" s="106"/>
+      <c r="W13" s="106"/>
+      <c r="X13" s="22"/>
+      <c r="Y13" s="22"/>
+      <c r="Z13" s="22"/>
+      <c r="AA13" s="22"/>
+      <c r="AB13" s="22"/>
+      <c r="AC13" s="22"/>
+      <c r="AD13" s="22"/>
+      <c r="AE13" s="22"/>
+      <c r="AF13" s="22"/>
+      <c r="AG13" s="22"/>
     </row>
     <row r="14" spans="1:47" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
@@ -2287,6 +2475,23 @@
       </c>
       <c r="O14" s="22"/>
       <c r="P14" s="52"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="106"/>
+      <c r="U14" s="106"/>
+      <c r="V14" s="106"/>
+      <c r="W14" s="106"/>
+      <c r="X14" s="22"/>
+      <c r="Y14" s="22"/>
+      <c r="Z14" s="22"/>
+      <c r="AA14" s="22"/>
+      <c r="AB14" s="22"/>
+      <c r="AC14" s="22"/>
+      <c r="AD14" s="22"/>
+      <c r="AE14" s="22"/>
+      <c r="AF14" s="22"/>
+      <c r="AG14" s="22"/>
     </row>
     <row r="15" spans="1:47" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
@@ -2307,6 +2512,23 @@
       <c r="N15" s="22"/>
       <c r="O15" s="22"/>
       <c r="P15" s="52"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="106"/>
+      <c r="U15" s="106"/>
+      <c r="V15" s="106"/>
+      <c r="W15" s="106"/>
+      <c r="X15" s="22"/>
+      <c r="Y15" s="22"/>
+      <c r="Z15" s="22"/>
+      <c r="AA15" s="22"/>
+      <c r="AB15" s="22"/>
+      <c r="AC15" s="22"/>
+      <c r="AD15" s="22"/>
+      <c r="AE15" s="22"/>
+      <c r="AF15" s="22"/>
+      <c r="AG15" s="22"/>
     </row>
     <row r="16" spans="1:47" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
@@ -2327,8 +2549,25 @@
       <c r="N16" s="22"/>
       <c r="O16" s="22"/>
       <c r="P16" s="52"/>
-    </row>
-    <row r="17" spans="1:16" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="106"/>
+      <c r="U16" s="106"/>
+      <c r="V16" s="106"/>
+      <c r="W16" s="106"/>
+      <c r="X16" s="22"/>
+      <c r="Y16" s="22"/>
+      <c r="Z16" s="22"/>
+      <c r="AA16" s="22"/>
+      <c r="AB16" s="22"/>
+      <c r="AC16" s="22"/>
+      <c r="AD16" s="22"/>
+      <c r="AE16" s="22"/>
+      <c r="AF16" s="22"/>
+      <c r="AG16" s="22"/>
+    </row>
+    <row r="17" spans="1:33" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="21"/>
       <c r="C17" s="22"/>
@@ -2345,8 +2584,25 @@
       <c r="N17" s="22"/>
       <c r="O17" s="22"/>
       <c r="P17" s="52"/>
-    </row>
-    <row r="18" spans="1:16" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="106"/>
+      <c r="U17" s="106"/>
+      <c r="V17" s="106"/>
+      <c r="W17" s="106"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
+      <c r="AG17" s="22"/>
+    </row>
+    <row r="18" spans="1:33" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="21"/>
       <c r="C18" s="22"/>
@@ -2363,8 +2619,25 @@
       <c r="N18" s="22"/>
       <c r="O18" s="22"/>
       <c r="P18" s="52"/>
-    </row>
-    <row r="19" spans="1:16" s="37" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="106"/>
+      <c r="U18" s="106"/>
+      <c r="V18" s="106"/>
+      <c r="W18" s="106"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22"/>
+      <c r="Z18" s="22"/>
+      <c r="AA18" s="22"/>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="22"/>
+      <c r="AD18" s="22"/>
+      <c r="AE18" s="22"/>
+      <c r="AF18" s="22"/>
+      <c r="AG18" s="22"/>
+    </row>
+    <row r="19" spans="1:33" s="37" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="28"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
@@ -2381,8 +2654,25 @@
       <c r="N19" s="36"/>
       <c r="O19" s="36"/>
       <c r="P19" s="52"/>
-    </row>
-    <row r="20" spans="1:16" s="41" customFormat="1" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="107"/>
+      <c r="U19" s="107"/>
+      <c r="V19" s="107"/>
+      <c r="W19" s="107"/>
+      <c r="X19" s="36"/>
+      <c r="Y19" s="36"/>
+      <c r="Z19" s="36"/>
+      <c r="AA19" s="36"/>
+      <c r="AB19" s="36"/>
+      <c r="AC19" s="36"/>
+      <c r="AD19" s="36"/>
+      <c r="AE19" s="36"/>
+      <c r="AF19" s="36"/>
+      <c r="AG19" s="36"/>
+    </row>
+    <row r="20" spans="1:33" s="41" customFormat="1" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="38" t="s">
         <v>1</v>
       </c>
@@ -2424,9 +2714,23 @@
       <c r="M20" s="40"/>
       <c r="N20" s="40"/>
       <c r="O20" s="40"/>
-      <c r="P20" s="52"/>
-    </row>
-    <row r="21" spans="1:16" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="P20" s="53"/>
+      <c r="Q20" s="40">
+        <v>2</v>
+      </c>
+      <c r="R20" s="41">
+        <v>3</v>
+      </c>
+      <c r="S20" s="40">
+        <v>2</v>
+      </c>
+      <c r="T20" s="53"/>
+      <c r="U20" s="53"/>
+      <c r="V20" s="53"/>
+      <c r="W20" s="53"/>
+      <c r="X20" s="40"/>
+    </row>
+    <row r="21" spans="1:33" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B21" s="101">
         <f>HOUR(B4)</f>
         <v>8</v>
@@ -2475,30 +2779,69 @@
         <f t="shared" ref="M21:O21" si="3">HOUR(M4)</f>
         <v>9</v>
       </c>
-      <c r="N21" s="101" t="e">
+      <c r="N21" s="101">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="O21" s="101" t="e">
+        <v>11</v>
+      </c>
+      <c r="O21" s="101">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="P21" s="95">
+        <f>SUM(L21:O21)</f>
+        <v>39</v>
+      </c>
+      <c r="Q21" s="101">
+        <f t="shared" ref="Q21:AA21" si="4">HOUR(Q4)</f>
+        <v>9</v>
+      </c>
+      <c r="R21" s="101">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="S21" s="101">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="T21" s="95">
+        <f>SUM(Q21:S21)</f>
+        <v>22</v>
+      </c>
+      <c r="U21" s="95"/>
+      <c r="V21" s="95"/>
+      <c r="W21" s="95"/>
+      <c r="X21" s="101">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y21" s="101">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="101">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="101">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="101">
         <f>MINUTE(B4)</f>
         <v>12</v>
       </c>
       <c r="C22" s="101">
-        <f t="shared" ref="C22:E22" si="4">MINUTE(C4)</f>
+        <f t="shared" ref="C22:E22" si="5">MINUTE(C4)</f>
         <v>0</v>
       </c>
       <c r="D22" s="101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="E22" s="101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="F22" s="95">
@@ -2506,19 +2849,19 @@
         <v>40</v>
       </c>
       <c r="G22" s="101">
-        <f t="shared" ref="G22:J22" si="5">MINUTE(G4)</f>
+        <f t="shared" ref="G22:J22" si="6">MINUTE(G4)</f>
         <v>41</v>
       </c>
       <c r="H22" s="101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>56</v>
       </c>
       <c r="I22" s="101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="J22" s="101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="K22" s="95">
@@ -2530,19 +2873,61 @@
         <v>12</v>
       </c>
       <c r="M22" s="101">
-        <f t="shared" ref="M22:O22" si="6">MINUTE(M4)</f>
+        <f t="shared" ref="M22:O22" si="7">MINUTE(M4)</f>
         <v>30</v>
       </c>
-      <c r="N22" s="101" t="e">
-        <f t="shared" si="6"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="O22" s="101" t="e">
-        <f t="shared" si="6"/>
-        <v>#NUM!</v>
+      <c r="N22" s="101">
+        <f t="shared" si="7"/>
+        <v>22</v>
+      </c>
+      <c r="O22" s="101">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="P22" s="95">
+        <f>SUM(L22:O22)</f>
+        <v>68</v>
+      </c>
+      <c r="Q22" s="101">
+        <f t="shared" ref="Q22:AA22" si="8">MINUTE(Q4)</f>
+        <v>36</v>
+      </c>
+      <c r="R22" s="101">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="S22" s="101">
+        <f t="shared" si="8"/>
+        <v>52</v>
+      </c>
+      <c r="T22" s="95">
+        <f>SUM(Q22:S22)</f>
+        <v>123</v>
+      </c>
+      <c r="U22" s="95"/>
+      <c r="V22" s="95"/>
+      <c r="W22" s="95"/>
+      <c r="X22" s="101">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="101">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="101">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="101">
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="T2:W19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2550,10 +2935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS31"/>
+  <dimension ref="A1:AP31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.28515625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2575,11 +2960,13 @@
     <col min="15" max="15" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.85546875" style="1" customWidth="1"/>
     <col min="17" max="17" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="45" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="16384" width="32.28515625" style="1"/>
+    <col min="18" max="19" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" style="1" customWidth="1"/>
+    <col min="21" max="42" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="16384" width="32.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="60" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="60" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="63"/>
       <c r="B1" s="61">
         <v>44753</v>
@@ -2635,86 +3022,77 @@
       <c r="S1" s="67">
         <v>44776</v>
       </c>
-      <c r="T1" s="67">
-        <v>44777</v>
+      <c r="T1" s="67" t="s">
+        <v>125</v>
       </c>
       <c r="U1" s="67">
-        <v>44778</v>
+        <v>44781</v>
       </c>
       <c r="V1" s="67">
-        <v>44779</v>
+        <v>44782</v>
       </c>
       <c r="W1" s="67">
-        <v>44780</v>
+        <v>44783</v>
       </c>
       <c r="X1" s="67">
-        <v>44781</v>
+        <v>44784</v>
       </c>
       <c r="Y1" s="67">
-        <v>44782</v>
+        <v>44785</v>
       </c>
       <c r="Z1" s="67">
-        <v>44783</v>
+        <v>44786</v>
       </c>
       <c r="AA1" s="67">
-        <v>44784</v>
+        <v>44787</v>
       </c>
       <c r="AB1" s="67">
-        <v>44785</v>
+        <v>44788</v>
       </c>
       <c r="AC1" s="67">
-        <v>44786</v>
-      </c>
-      <c r="AD1" s="67">
-        <v>44787</v>
-      </c>
-      <c r="AE1" s="67">
-        <v>44788</v>
-      </c>
-      <c r="AF1" s="67">
         <v>44789</v>
       </c>
+      <c r="AD1" s="60">
+        <v>44790</v>
+      </c>
+      <c r="AE1" s="60">
+        <v>44791</v>
+      </c>
+      <c r="AF1" s="60">
+        <v>44792</v>
+      </c>
       <c r="AG1" s="60">
-        <v>44790</v>
+        <v>44793</v>
       </c>
       <c r="AH1" s="60">
-        <v>44791</v>
+        <v>44794</v>
       </c>
       <c r="AI1" s="60">
-        <v>44792</v>
+        <v>44795</v>
       </c>
       <c r="AJ1" s="60">
-        <v>44793</v>
+        <v>44796</v>
       </c>
       <c r="AK1" s="60">
-        <v>44794</v>
+        <v>44797</v>
       </c>
       <c r="AL1" s="60">
-        <v>44795</v>
+        <v>44798</v>
       </c>
       <c r="AM1" s="60">
-        <v>44796</v>
+        <v>44799</v>
       </c>
       <c r="AN1" s="60">
-        <v>44797</v>
+        <v>44800</v>
       </c>
       <c r="AO1" s="60">
-        <v>44798</v>
+        <v>44801</v>
       </c>
       <c r="AP1" s="60">
-        <v>44799</v>
-      </c>
-      <c r="AQ1" s="60">
-        <v>44800</v>
-      </c>
-      <c r="AR1" s="60">
-        <v>44801</v>
-      </c>
-      <c r="AS1" s="60">
         <v>44802</v>
       </c>
     </row>
-    <row r="2" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="91">
         <v>0.33333333333333331</v>
       </c>
@@ -2735,8 +3113,10 @@
       <c r="P2" s="99"/>
       <c r="Q2" s="99"/>
       <c r="R2" s="99"/>
-    </row>
-    <row r="3" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S2" s="99"/>
+      <c r="T2" s="99"/>
+    </row>
+    <row r="3" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="91">
         <v>0.35416666666666669</v>
       </c>
@@ -2763,21 +3143,23 @@
       <c r="P3" s="99"/>
       <c r="Q3" s="99"/>
       <c r="R3" s="99"/>
-    </row>
-    <row r="4" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S3" s="99"/>
+      <c r="T3" s="99"/>
+    </row>
+    <row r="4" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="91">
         <v>0.375</v>
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="93"/>
-      <c r="D4" s="105" t="s">
+      <c r="D4" s="109" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="71" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="82"/>
-      <c r="G4" s="105" t="s">
+      <c r="G4" s="109" t="s">
         <v>53</v>
       </c>
       <c r="H4" s="69" t="s">
@@ -2801,36 +3183,38 @@
         <v>28</v>
       </c>
       <c r="R4" s="99"/>
-    </row>
-    <row r="5" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S4" s="99"/>
+      <c r="T4" s="99"/>
+    </row>
+    <row r="5" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="91">
         <v>0.39583333333333298</v>
       </c>
       <c r="B5" s="71"/>
       <c r="C5" s="93"/>
-      <c r="D5" s="107"/>
+      <c r="D5" s="111"/>
       <c r="E5" s="71" t="s">
         <v>41</v>
       </c>
       <c r="F5" s="82"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="105" t="s">
+      <c r="G5" s="111"/>
+      <c r="H5" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="105" t="s">
+      <c r="I5" s="109" t="s">
         <v>28</v>
       </c>
       <c r="J5" s="72" t="s">
         <v>78</v>
       </c>
       <c r="K5" s="65"/>
-      <c r="L5" s="104" t="s">
+      <c r="L5" s="108" t="s">
         <v>74</v>
       </c>
       <c r="M5" s="96" t="s">
         <v>93</v>
       </c>
-      <c r="N5" s="104" t="s">
+      <c r="N5" s="108" t="s">
         <v>95</v>
       </c>
       <c r="O5" s="96" t="s">
@@ -2838,8 +3222,12 @@
       </c>
       <c r="P5" s="99"/>
       <c r="R5" s="99"/>
-    </row>
-    <row r="6" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" s="99"/>
+    </row>
+    <row r="6" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="91">
         <v>0.41666666666666702</v>
       </c>
@@ -2847,23 +3235,23 @@
       <c r="C6" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="106"/>
-      <c r="E6" s="105" t="s">
+      <c r="D6" s="110"/>
+      <c r="E6" s="109" t="s">
         <v>46</v>
       </c>
       <c r="F6" s="82"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="106"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="110"/>
       <c r="J6" s="72" t="s">
         <v>79</v>
       </c>
       <c r="K6" s="65"/>
-      <c r="L6" s="104"/>
-      <c r="M6" s="104" t="s">
+      <c r="L6" s="108"/>
+      <c r="M6" s="108" t="s">
         <v>96</v>
       </c>
-      <c r="N6" s="104"/>
+      <c r="N6" s="108"/>
       <c r="O6" s="96" t="s">
         <v>106</v>
       </c>
@@ -2871,8 +3259,12 @@
       <c r="R6" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S6" s="108" t="s">
+        <v>124</v>
+      </c>
+      <c r="T6" s="99"/>
+    </row>
+    <row r="7" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="91">
         <v>0.4375</v>
       </c>
@@ -2883,10 +3275,10 @@
       <c r="D7" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="107"/>
+      <c r="E7" s="111"/>
       <c r="F7" s="82"/>
-      <c r="G7" s="107"/>
-      <c r="H7" s="107"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
       <c r="I7" s="72" t="s">
         <v>69</v>
       </c>
@@ -2894,15 +3286,17 @@
         <v>80</v>
       </c>
       <c r="K7" s="65"/>
-      <c r="L7" s="104"/>
-      <c r="M7" s="104"/>
-      <c r="N7" s="104"/>
-      <c r="O7" s="104" t="s">
+      <c r="L7" s="108"/>
+      <c r="M7" s="108"/>
+      <c r="N7" s="108"/>
+      <c r="O7" s="108" t="s">
         <v>107</v>
       </c>
       <c r="P7" s="99"/>
-    </row>
-    <row r="8" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S7" s="108"/>
+      <c r="T7" s="99"/>
+    </row>
+    <row r="8" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="91">
         <v>0.45833333333333298</v>
       </c>
@@ -2910,13 +3304,13 @@
       <c r="C8" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="105" t="s">
+      <c r="D8" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="107"/>
+      <c r="E8" s="111"/>
       <c r="F8" s="82"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="106"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="110"/>
       <c r="I8" s="72" t="s">
         <v>70</v>
       </c>
@@ -2924,135 +3318,142 @@
         <v>81</v>
       </c>
       <c r="K8" s="65"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="104"/>
-      <c r="O8" s="104"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="108"/>
+      <c r="N8" s="108"/>
+      <c r="O8" s="108"/>
       <c r="P8" s="99"/>
-    </row>
-    <row r="9" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S8" s="108"/>
+      <c r="T8" s="99"/>
+    </row>
+    <row r="9" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="91">
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="71"/>
-      <c r="C9" s="108" t="s">
+      <c r="C9" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="107"/>
-      <c r="E9" s="106"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="110"/>
       <c r="F9" s="82"/>
       <c r="G9" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="105" t="s">
+      <c r="H9" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="105" t="s">
+      <c r="I9" s="109" t="s">
         <v>71</v>
       </c>
       <c r="J9" s="72" t="s">
         <v>73</v>
       </c>
       <c r="K9" s="65"/>
-      <c r="L9" s="104"/>
-      <c r="M9" s="104"/>
-      <c r="N9" s="104"/>
-      <c r="O9" s="104"/>
+      <c r="L9" s="108"/>
+      <c r="M9" s="108"/>
+      <c r="N9" s="108"/>
+      <c r="O9" s="108"/>
       <c r="P9" s="99"/>
-    </row>
-    <row r="10" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S9" s="108"/>
+      <c r="T9" s="99"/>
+    </row>
+    <row r="10" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="91">
         <v>0.5</v>
       </c>
       <c r="B10" s="71"/>
-      <c r="C10" s="108"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="105" t="s">
+      <c r="C10" s="112"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="109" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="82"/>
-      <c r="G10" s="105" t="s">
+      <c r="G10" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="107"/>
-      <c r="I10" s="107"/>
-      <c r="J10" s="105" t="s">
+      <c r="H10" s="111"/>
+      <c r="I10" s="111"/>
+      <c r="J10" s="109" t="s">
         <v>82</v>
       </c>
       <c r="K10" s="65"/>
-      <c r="L10" s="104"/>
-      <c r="M10" s="104"/>
-      <c r="N10" s="104"/>
+      <c r="L10" s="108"/>
+      <c r="M10" s="108"/>
+      <c r="N10" s="108"/>
       <c r="O10" s="96" t="s">
         <v>15</v>
       </c>
       <c r="P10" s="99"/>
-      <c r="Q10" s="104" t="s">
+      <c r="Q10" s="108" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T10" s="99"/>
+    </row>
+    <row r="11" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="91">
         <v>0.52083333333333304</v>
       </c>
       <c r="B11" s="71"/>
-      <c r="C11" s="108"/>
-      <c r="D11" s="107"/>
-      <c r="E11" s="106"/>
+      <c r="C11" s="112"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="110"/>
       <c r="F11" s="82"/>
-      <c r="G11" s="107"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="107"/>
-      <c r="J11" s="107"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="111"/>
+      <c r="I11" s="111"/>
+      <c r="J11" s="111"/>
       <c r="K11" s="65"/>
-      <c r="L11" s="104"/>
+      <c r="L11" s="108"/>
       <c r="M11" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="N11" s="104" t="s">
+      <c r="N11" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="O11" s="104" t="s">
+      <c r="O11" s="108" t="s">
         <v>109</v>
       </c>
       <c r="P11" s="99"/>
-      <c r="Q11" s="104"/>
-    </row>
-    <row r="12" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q11" s="108"/>
+      <c r="T11" s="99"/>
+    </row>
+    <row r="12" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="91">
         <v>0.54166666666666696</v>
       </c>
       <c r="B12" s="71"/>
-      <c r="C12" s="108" t="s">
+      <c r="C12" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="106"/>
+      <c r="D12" s="110"/>
       <c r="E12" s="71" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="82"/>
-      <c r="G12" s="106"/>
-      <c r="H12" s="107"/>
-      <c r="I12" s="107"/>
-      <c r="J12" s="106"/>
+      <c r="G12" s="110"/>
+      <c r="H12" s="111"/>
+      <c r="I12" s="111"/>
+      <c r="J12" s="110"/>
       <c r="K12" s="65"/>
-      <c r="L12" s="104" t="s">
+      <c r="L12" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="M12" s="104" t="s">
+      <c r="M12" s="108" t="s">
         <v>95</v>
       </c>
-      <c r="N12" s="104"/>
-      <c r="O12" s="104"/>
+      <c r="N12" s="108"/>
+      <c r="O12" s="108"/>
       <c r="P12" s="99"/>
-    </row>
-    <row r="13" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T12" s="99"/>
+    </row>
+    <row r="13" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="91">
         <v>0.5625</v>
       </c>
       <c r="B13" s="71"/>
-      <c r="C13" s="108"/>
-      <c r="D13" s="105" t="s">
+      <c r="C13" s="112"/>
+      <c r="D13" s="109" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="71" t="s">
@@ -3062,159 +3463,165 @@
       <c r="G13" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="106"/>
-      <c r="I13" s="107"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="111"/>
       <c r="J13" s="72" t="s">
         <v>84</v>
       </c>
       <c r="K13" s="65"/>
-      <c r="L13" s="104"/>
-      <c r="M13" s="104"/>
-      <c r="N13" s="104" t="s">
+      <c r="L13" s="108"/>
+      <c r="M13" s="108"/>
+      <c r="N13" s="108" t="s">
         <v>105</v>
       </c>
-      <c r="O13" s="104"/>
+      <c r="O13" s="108"/>
       <c r="P13" s="99"/>
-    </row>
-    <row r="14" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T13" s="99"/>
+    </row>
+    <row r="14" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="91">
         <v>0.58333333333333304</v>
       </c>
       <c r="B14" s="71"/>
-      <c r="C14" s="108" t="s">
+      <c r="C14" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="106"/>
-      <c r="E14" s="105" t="s">
+      <c r="D14" s="110"/>
+      <c r="E14" s="109" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="82"/>
       <c r="G14" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="105" t="s">
+      <c r="H14" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="106"/>
-      <c r="J14" s="105" t="s">
+      <c r="I14" s="110"/>
+      <c r="J14" s="109" t="s">
         <v>15</v>
       </c>
       <c r="K14" s="65"/>
-      <c r="L14" s="104" t="s">
+      <c r="L14" s="108" t="s">
         <v>91</v>
       </c>
-      <c r="M14" s="104"/>
-      <c r="N14" s="104"/>
-      <c r="O14" s="104"/>
+      <c r="M14" s="108"/>
+      <c r="N14" s="108"/>
+      <c r="O14" s="108"/>
       <c r="P14" s="99"/>
-    </row>
-    <row r="15" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T14" s="99"/>
+    </row>
+    <row r="15" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="91">
         <v>0.60416666666666696</v>
       </c>
       <c r="B15" s="71"/>
-      <c r="C15" s="108"/>
-      <c r="D15" s="105" t="s">
+      <c r="C15" s="112"/>
+      <c r="D15" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="106"/>
+      <c r="E15" s="110"/>
       <c r="F15" s="82"/>
-      <c r="G15" s="105" t="s">
+      <c r="G15" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="H15" s="107"/>
+      <c r="H15" s="111"/>
       <c r="I15" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="106"/>
+      <c r="J15" s="110"/>
       <c r="K15" s="65"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="104"/>
-      <c r="O15" s="104"/>
+      <c r="L15" s="108"/>
+      <c r="M15" s="108"/>
+      <c r="N15" s="108"/>
+      <c r="O15" s="108"/>
       <c r="P15" s="99"/>
-    </row>
-    <row r="16" spans="1:45" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T15" s="99"/>
+    </row>
+    <row r="16" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="91">
         <v>0.625</v>
       </c>
       <c r="B16" s="71"/>
-      <c r="C16" s="108" t="s">
+      <c r="C16" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="106"/>
-      <c r="E16" s="105" t="s">
+      <c r="D16" s="110"/>
+      <c r="E16" s="109" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="82"/>
-      <c r="G16" s="107"/>
-      <c r="H16" s="106"/>
-      <c r="I16" s="105" t="s">
+      <c r="G16" s="111"/>
+      <c r="H16" s="110"/>
+      <c r="I16" s="109" t="s">
         <v>72</v>
       </c>
       <c r="J16" s="72" t="s">
         <v>85</v>
       </c>
       <c r="K16" s="65"/>
-      <c r="L16" s="104"/>
-      <c r="M16" s="104"/>
-      <c r="N16" s="104"/>
-      <c r="O16" s="104"/>
+      <c r="L16" s="108"/>
+      <c r="M16" s="108"/>
+      <c r="N16" s="108"/>
+      <c r="O16" s="108"/>
       <c r="P16" s="99"/>
-    </row>
-    <row r="17" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T16" s="99"/>
+    </row>
+    <row r="17" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="91">
         <v>0.64583333333333404</v>
       </c>
       <c r="B17" s="71"/>
-      <c r="C17" s="108"/>
-      <c r="D17" s="105" t="s">
+      <c r="C17" s="112"/>
+      <c r="D17" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="106"/>
+      <c r="E17" s="110"/>
       <c r="F17" s="82"/>
-      <c r="G17" s="107"/>
-      <c r="H17" s="105" t="s">
+      <c r="G17" s="111"/>
+      <c r="H17" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="I17" s="107"/>
-      <c r="J17" s="105" t="s">
+      <c r="I17" s="111"/>
+      <c r="J17" s="109" t="s">
         <v>86</v>
       </c>
       <c r="K17" s="65"/>
-      <c r="L17" s="104"/>
-      <c r="M17" s="104"/>
-      <c r="N17" s="104"/>
-      <c r="O17" s="104"/>
+      <c r="L17" s="108"/>
+      <c r="M17" s="108"/>
+      <c r="N17" s="108"/>
+      <c r="O17" s="108"/>
       <c r="P17" s="99"/>
-    </row>
-    <row r="18" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T17" s="99"/>
+    </row>
+    <row r="18" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="91">
         <v>0.66666666666666696</v>
       </c>
       <c r="B18" s="71"/>
-      <c r="C18" s="108"/>
-      <c r="D18" s="106"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="110"/>
       <c r="E18" s="71" t="s">
         <v>21</v>
       </c>
       <c r="F18" s="82"/>
-      <c r="G18" s="107"/>
-      <c r="H18" s="107"/>
-      <c r="I18" s="106"/>
-      <c r="J18" s="107"/>
+      <c r="G18" s="111"/>
+      <c r="H18" s="111"/>
+      <c r="I18" s="110"/>
+      <c r="J18" s="111"/>
       <c r="K18" s="65"/>
-      <c r="L18" s="104"/>
-      <c r="M18" s="104" t="s">
+      <c r="L18" s="108"/>
+      <c r="M18" s="108" t="s">
         <v>99</v>
       </c>
-      <c r="N18" s="104"/>
-      <c r="O18" s="104" t="s">
+      <c r="N18" s="108"/>
+      <c r="O18" s="108" t="s">
         <v>110</v>
       </c>
       <c r="P18" s="99"/>
-    </row>
-    <row r="19" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T18" s="99"/>
+    </row>
+    <row r="19" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="91">
         <v>0.6875</v>
       </c>
@@ -3225,26 +3632,27 @@
       <c r="D19" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="105" t="s">
+      <c r="E19" s="109" t="s">
         <v>48</v>
       </c>
       <c r="F19" s="82"/>
-      <c r="G19" s="107"/>
-      <c r="H19" s="107"/>
-      <c r="I19" s="105" t="s">
+      <c r="G19" s="111"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="109" t="s">
         <v>73</v>
       </c>
-      <c r="J19" s="107"/>
+      <c r="J19" s="111"/>
       <c r="K19" s="65"/>
-      <c r="L19" s="104"/>
-      <c r="M19" s="104"/>
+      <c r="L19" s="108"/>
+      <c r="M19" s="108"/>
       <c r="N19" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="104"/>
+      <c r="O19" s="108"/>
       <c r="P19" s="99"/>
-    </row>
-    <row r="20" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T19" s="99"/>
+    </row>
+    <row r="20" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="91">
         <v>0.70833333333333404</v>
       </c>
@@ -3252,75 +3660,79 @@
       <c r="C20" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="105" t="s">
+      <c r="D20" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="106"/>
+      <c r="E20" s="110"/>
       <c r="F20" s="82"/>
-      <c r="G20" s="107"/>
-      <c r="H20" s="107"/>
-      <c r="I20" s="106"/>
-      <c r="J20" s="107"/>
+      <c r="G20" s="111"/>
+      <c r="H20" s="111"/>
+      <c r="I20" s="110"/>
+      <c r="J20" s="111"/>
       <c r="K20" s="65"/>
       <c r="L20" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="M20" s="104" t="s">
+      <c r="M20" s="108" t="s">
         <v>95</v>
       </c>
       <c r="N20" s="96"/>
-      <c r="O20" s="104"/>
+      <c r="O20" s="108"/>
       <c r="P20" s="99"/>
-    </row>
-    <row r="21" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S20" s="98"/>
+      <c r="T20" s="98"/>
+    </row>
+    <row r="21" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="91">
         <v>0.72916666666666696</v>
       </c>
       <c r="B21" s="71"/>
-      <c r="C21" s="108" t="s">
+      <c r="C21" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="106"/>
+      <c r="D21" s="110"/>
       <c r="E21" s="71" t="s">
         <v>36</v>
       </c>
       <c r="F21" s="82"/>
-      <c r="G21" s="107"/>
-      <c r="H21" s="106"/>
-      <c r="I21" s="105" t="s">
+      <c r="G21" s="111"/>
+      <c r="H21" s="110"/>
+      <c r="I21" s="109" t="s">
         <v>70</v>
       </c>
-      <c r="J21" s="106"/>
+      <c r="J21" s="110"/>
       <c r="K21" s="65"/>
-      <c r="L21" s="104" t="s">
+      <c r="L21" s="108" t="s">
         <v>91</v>
       </c>
-      <c r="M21" s="104"/>
+      <c r="M21" s="108"/>
       <c r="N21" s="96"/>
       <c r="O21" s="96"/>
       <c r="P21" s="99"/>
-    </row>
-    <row r="22" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S21" s="98"/>
+      <c r="T21" s="98"/>
+    </row>
+    <row r="22" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="91">
         <v>0.75</v>
       </c>
       <c r="B22" s="71"/>
-      <c r="C22" s="108"/>
+      <c r="C22" s="112"/>
       <c r="D22" s="71" t="s">
         <v>37</v>
       </c>
       <c r="E22" s="64"/>
       <c r="F22" s="82"/>
-      <c r="G22" s="107"/>
+      <c r="G22" s="111"/>
       <c r="H22" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="106"/>
+      <c r="I22" s="110"/>
       <c r="J22" s="72" t="s">
         <v>87</v>
       </c>
       <c r="K22" s="65"/>
-      <c r="L22" s="104"/>
+      <c r="L22" s="108"/>
       <c r="M22" s="99"/>
       <c r="N22" s="96"/>
       <c r="O22" s="96"/>
@@ -3328,35 +3740,40 @@
       <c r="Q22" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S22" s="98"/>
+      <c r="T22" s="98"/>
+    </row>
+    <row r="23" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="91">
         <v>0.77083333333333404</v>
       </c>
       <c r="B23" s="71"/>
-      <c r="C23" s="108"/>
+      <c r="C23" s="112"/>
       <c r="D23" s="71" t="s">
         <v>36</v>
       </c>
       <c r="E23" s="64"/>
       <c r="F23" s="82"/>
-      <c r="G23" s="106"/>
+      <c r="G23" s="110"/>
       <c r="H23" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="I23" s="105" t="s">
+      <c r="I23" s="109" t="s">
         <v>74</v>
       </c>
       <c r="J23" s="64"/>
       <c r="K23" s="65"/>
-      <c r="L23" s="104"/>
+      <c r="L23" s="108"/>
       <c r="M23" s="99"/>
       <c r="N23" s="96"/>
       <c r="O23" s="96"/>
       <c r="P23" s="99"/>
       <c r="Q23" s="98"/>
-    </row>
-    <row r="24" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R23"/>
+      <c r="S23" s="98"/>
+      <c r="T23" s="98"/>
+    </row>
+    <row r="24" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="91">
         <v>0.79166666666666696</v>
       </c>
@@ -3369,7 +3786,7 @@
       <c r="F24" s="82"/>
       <c r="G24" s="64"/>
       <c r="H24" s="64"/>
-      <c r="I24" s="106"/>
+      <c r="I24" s="110"/>
       <c r="J24" s="64"/>
       <c r="K24" s="65"/>
       <c r="L24" s="96" t="s">
@@ -3380,8 +3797,11 @@
       <c r="O24" s="98"/>
       <c r="P24" s="98"/>
       <c r="Q24" s="98"/>
-    </row>
-    <row r="25" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R24" s="98"/>
+      <c r="S24" s="98"/>
+      <c r="T24" s="98"/>
+    </row>
+    <row r="25" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="91">
         <v>0.8125</v>
       </c>
@@ -3401,8 +3821,11 @@
       <c r="O25" s="98"/>
       <c r="P25" s="98"/>
       <c r="Q25" s="98"/>
-    </row>
-    <row r="26" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R25" s="98"/>
+      <c r="S25" s="98"/>
+      <c r="T25" s="98"/>
+    </row>
+    <row r="26" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="91">
         <v>0.83333333333333304</v>
       </c>
@@ -3422,8 +3845,11 @@
       <c r="O26" s="98"/>
       <c r="P26" s="98"/>
       <c r="Q26" s="98"/>
-    </row>
-    <row r="27" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R26" s="98"/>
+      <c r="S26" s="98"/>
+      <c r="T26" s="98"/>
+    </row>
+    <row r="27" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="91">
         <v>0.85416666666666596</v>
       </c>
@@ -3443,8 +3869,11 @@
       <c r="O27" s="98"/>
       <c r="P27" s="98"/>
       <c r="Q27" s="98"/>
-    </row>
-    <row r="28" spans="1:17" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R27" s="98"/>
+      <c r="S27" s="98"/>
+      <c r="T27" s="98"/>
+    </row>
+    <row r="28" spans="1:20" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="91">
         <v>0.874999999999999</v>
       </c>
@@ -3463,21 +3892,23 @@
       <c r="O28" s="98"/>
       <c r="P28" s="98"/>
       <c r="Q28" s="98"/>
-    </row>
-    <row r="29" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R28" s="98"/>
+      <c r="S28" s="98"/>
+      <c r="T28" s="98"/>
+    </row>
+    <row r="29" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="89"/>
       <c r="E29" s="89"/>
       <c r="F29" s="76"/>
     </row>
-    <row r="30" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F30" s="76"/>
     </row>
-    <row r="31" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F31" s="76"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
-    <mergeCell ref="I5:I6"/>
+  <mergeCells count="48">
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="I9:I14"/>
     <mergeCell ref="I16:I18"/>
@@ -3488,30 +3919,28 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="H5:H8"/>
     <mergeCell ref="E19:E20"/>
-    <mergeCell ref="G4:G8"/>
     <mergeCell ref="G10:G12"/>
-    <mergeCell ref="N5:N10"/>
-    <mergeCell ref="H9:H13"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="H17:H21"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
     <mergeCell ref="G15:G23"/>
     <mergeCell ref="E6:E9"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="E16:E17"/>
+    <mergeCell ref="G4:G8"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="N5:N10"/>
+    <mergeCell ref="H9:H13"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="H17:H21"/>
     <mergeCell ref="N13:N18"/>
-    <mergeCell ref="Q10:Q11"/>
-    <mergeCell ref="O7:O9"/>
-    <mergeCell ref="O11:O17"/>
-    <mergeCell ref="O18:O20"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="H5:H8"/>
     <mergeCell ref="I23:I24"/>
     <mergeCell ref="M6:M10"/>
     <mergeCell ref="M12:M17"/>
@@ -3523,7 +3952,11 @@
     <mergeCell ref="L5:L11"/>
     <mergeCell ref="I19:I20"/>
     <mergeCell ref="I21:I22"/>
-    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="S6:S9"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="O7:O9"/>
+    <mergeCell ref="O11:O17"/>
+    <mergeCell ref="O18:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3534,7 +3967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: workload dump WIP!
</commit_message>
<xml_diff>
--- a/__docs/diary.xlsx
+++ b/__docs/diary.xlsx
@@ -17,6 +17,7 @@
     <sheet name="Napi terv" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="126">
   <si>
     <t>Felmerült problémák:</t>
   </si>
@@ -1543,8 +1544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:W19"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1765,7 +1766,9 @@
       <c r="U2" s="106"/>
       <c r="V2" s="106"/>
       <c r="W2" s="106"/>
-      <c r="X2" s="13"/>
+      <c r="X2" s="13">
+        <v>0.36180555555555555</v>
+      </c>
       <c r="Y2" s="13"/>
       <c r="Z2" s="13"/>
       <c r="AA2" s="13"/>
@@ -1950,9 +1953,9 @@
       <c r="U4" s="106"/>
       <c r="V4" s="106"/>
       <c r="W4" s="106"/>
-      <c r="X4" s="36">
+      <c r="X4" s="105">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.36180555555555555</v>
       </c>
       <c r="Y4" s="36">
         <f t="shared" si="0"/>
@@ -2736,15 +2739,15 @@
         <v>8</v>
       </c>
       <c r="C21" s="101">
-        <f t="shared" ref="C21:E21" si="1">HOUR(C4)</f>
+        <f>HOUR(C4)</f>
         <v>10</v>
       </c>
       <c r="D21" s="101">
-        <f t="shared" si="1"/>
+        <f>HOUR(D4)</f>
         <v>10</v>
       </c>
       <c r="E21" s="101">
-        <f t="shared" si="1"/>
+        <f>HOUR(E4)</f>
         <v>9</v>
       </c>
       <c r="F21" s="95">
@@ -2752,19 +2755,19 @@
         <v>37</v>
       </c>
       <c r="G21" s="101">
-        <f t="shared" ref="G21:J21" si="2">HOUR(G4)</f>
+        <f>HOUR(G4)</f>
         <v>10</v>
       </c>
       <c r="H21" s="101">
-        <f t="shared" si="2"/>
+        <f>HOUR(H4)</f>
         <v>9</v>
       </c>
       <c r="I21" s="101">
-        <f t="shared" si="2"/>
+        <f>HOUR(I4)</f>
         <v>10</v>
       </c>
       <c r="J21" s="101">
-        <f t="shared" si="2"/>
+        <f>HOUR(J4)</f>
         <v>9</v>
       </c>
       <c r="K21" s="95">
@@ -2776,15 +2779,15 @@
         <v>10</v>
       </c>
       <c r="M21" s="101">
-        <f t="shared" ref="M21:O21" si="3">HOUR(M4)</f>
+        <f>HOUR(M4)</f>
         <v>9</v>
       </c>
       <c r="N21" s="101">
-        <f t="shared" si="3"/>
+        <f>HOUR(N4)</f>
         <v>11</v>
       </c>
       <c r="O21" s="101">
-        <f t="shared" si="3"/>
+        <f>HOUR(O4)</f>
         <v>9</v>
       </c>
       <c r="P21" s="95">
@@ -2792,15 +2795,15 @@
         <v>39</v>
       </c>
       <c r="Q21" s="101">
-        <f t="shared" ref="Q21:AA21" si="4">HOUR(Q4)</f>
+        <f t="shared" ref="Q21:AA21" si="1">HOUR(Q4)</f>
         <v>9</v>
       </c>
       <c r="R21" s="101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="S21" s="101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="T21" s="95">
@@ -2810,20 +2813,20 @@
       <c r="U21" s="95"/>
       <c r="V21" s="95"/>
       <c r="W21" s="95"/>
-      <c r="X21" s="101">
-        <f t="shared" si="4"/>
+      <c r="X21" s="101" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Y21" s="101">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Y21" s="101">
-        <f t="shared" si="4"/>
+      <c r="Z21" s="101">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z21" s="101">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="AA21" s="101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2833,15 +2836,15 @@
         <v>12</v>
       </c>
       <c r="C22" s="101">
-        <f t="shared" ref="C22:E22" si="5">MINUTE(C4)</f>
+        <f>MINUTE(C4)</f>
         <v>0</v>
       </c>
       <c r="D22" s="101">
-        <f t="shared" si="5"/>
+        <f>MINUTE(D4)</f>
         <v>20</v>
       </c>
       <c r="E22" s="101">
-        <f t="shared" si="5"/>
+        <f>MINUTE(E4)</f>
         <v>8</v>
       </c>
       <c r="F22" s="95">
@@ -2849,19 +2852,19 @@
         <v>40</v>
       </c>
       <c r="G22" s="101">
-        <f t="shared" ref="G22:J22" si="6">MINUTE(G4)</f>
+        <f>MINUTE(G4)</f>
         <v>41</v>
       </c>
       <c r="H22" s="101">
-        <f t="shared" si="6"/>
+        <f>MINUTE(H4)</f>
         <v>56</v>
       </c>
       <c r="I22" s="101">
-        <f t="shared" si="6"/>
+        <f>MINUTE(I4)</f>
         <v>3</v>
       </c>
       <c r="J22" s="101">
-        <f t="shared" si="6"/>
+        <f>MINUTE(J4)</f>
         <v>20</v>
       </c>
       <c r="K22" s="95">
@@ -2873,15 +2876,15 @@
         <v>12</v>
       </c>
       <c r="M22" s="101">
-        <f t="shared" ref="M22:O22" si="7">MINUTE(M4)</f>
+        <f>MINUTE(M4)</f>
         <v>30</v>
       </c>
       <c r="N22" s="101">
-        <f t="shared" si="7"/>
+        <f>MINUTE(N4)</f>
         <v>22</v>
       </c>
       <c r="O22" s="101">
-        <f t="shared" si="7"/>
+        <f>MINUTE(O4)</f>
         <v>4</v>
       </c>
       <c r="P22" s="95">
@@ -2889,15 +2892,15 @@
         <v>68</v>
       </c>
       <c r="Q22" s="101">
-        <f t="shared" ref="Q22:AA22" si="8">MINUTE(Q4)</f>
+        <f t="shared" ref="Q22:AA22" si="2">MINUTE(Q4)</f>
         <v>36</v>
       </c>
       <c r="R22" s="101">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="S22" s="101">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="T22" s="95">
@@ -2907,20 +2910,20 @@
       <c r="U22" s="95"/>
       <c r="V22" s="95"/>
       <c r="W22" s="95"/>
-      <c r="X22" s="101">
-        <f t="shared" si="8"/>
+      <c r="X22" s="101" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Y22" s="101">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y22" s="101">
-        <f t="shared" si="8"/>
+      <c r="Z22" s="101">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z22" s="101">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
       <c r="AA22" s="101">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2937,8 +2940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.28515625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3115,6 +3118,7 @@
       <c r="R2" s="99"/>
       <c r="S2" s="99"/>
       <c r="T2" s="99"/>
+      <c r="U2" s="99"/>
     </row>
     <row r="3" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="91">
@@ -3145,6 +3149,7 @@
       <c r="R3" s="99"/>
       <c r="S3" s="99"/>
       <c r="T3" s="99"/>
+      <c r="U3" s="99"/>
     </row>
     <row r="4" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="91">
@@ -3185,6 +3190,9 @@
       <c r="R4" s="99"/>
       <c r="S4" s="99"/>
       <c r="T4" s="99"/>
+      <c r="U4" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="91">

</xml_diff>

<commit_message>
feat: refine fish convex max
</commit_message>
<xml_diff>
--- a/__docs/diary.xlsx
+++ b/__docs/diary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9330"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1247,16 +1247,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1543,8 +1543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU22"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z6" sqref="Z6"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1778,7 +1778,9 @@
       <c r="Z2" s="13">
         <v>0.40208333333333335</v>
       </c>
-      <c r="AA2" s="13"/>
+      <c r="AA2" s="13">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="AB2" s="13"/>
       <c r="AC2" s="13"/>
       <c r="AD2" s="13"/>
@@ -1869,7 +1871,9 @@
       <c r="Y3" s="15">
         <v>0.84027777777777779</v>
       </c>
-      <c r="Z3" s="15"/>
+      <c r="Z3" s="15">
+        <v>0.81111111111111101</v>
+      </c>
       <c r="AA3" s="15"/>
       <c r="AB3" s="15"/>
       <c r="AC3" s="15"/>
@@ -1980,11 +1984,11 @@
       </c>
       <c r="Z4" s="103">
         <f t="shared" si="0"/>
-        <v>-0.40208333333333335</v>
+        <v>0.40902777777777766</v>
       </c>
       <c r="AA4" s="103">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.41666666666666669</v>
       </c>
       <c r="AB4" s="103">
         <f t="shared" si="0"/>
@@ -2840,13 +2844,13 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="Z21" s="99" t="e">
+      <c r="Z21" s="99">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="AA21" s="99" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
-      </c>
-      <c r="AA21" s="99">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -2937,13 +2941,13 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="Z22" s="99" t="e">
+      <c r="Z22" s="99">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="AA22" s="99" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
-      </c>
-      <c r="AA22" s="99">
-        <f t="shared" si="2"/>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2959,8 +2963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA17" sqref="AA17"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.28515625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3139,6 +3143,7 @@
       <c r="T2" s="97"/>
       <c r="U2" s="97"/>
       <c r="V2" s="97"/>
+      <c r="W2" s="97"/>
     </row>
     <row r="3" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89">
@@ -3171,6 +3176,7 @@
       <c r="T3" s="97"/>
       <c r="U3" s="97"/>
       <c r="V3" s="97"/>
+      <c r="W3" s="97"/>
     </row>
     <row r="4" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="89">
@@ -3178,14 +3184,14 @@
       </c>
       <c r="B4" s="69"/>
       <c r="C4" s="91"/>
-      <c r="D4" s="108" t="s">
+      <c r="D4" s="109" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="69" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="80"/>
-      <c r="G4" s="108" t="s">
+      <c r="G4" s="109" t="s">
         <v>53</v>
       </c>
       <c r="H4" s="67" t="s">
@@ -3215,6 +3221,7 @@
         <v>28</v>
       </c>
       <c r="V4" s="97"/>
+      <c r="W4" s="97"/>
     </row>
     <row r="5" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="89">
@@ -3228,10 +3235,10 @@
       </c>
       <c r="F5" s="80"/>
       <c r="G5" s="110"/>
-      <c r="H5" s="108" t="s">
+      <c r="H5" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="108" t="s">
+      <c r="I5" s="109" t="s">
         <v>28</v>
       </c>
       <c r="J5" s="70" t="s">
@@ -3257,6 +3264,7 @@
       </c>
       <c r="T5" s="97"/>
       <c r="V5" s="97"/>
+      <c r="W5" s="97"/>
     </row>
     <row r="6" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="89">
@@ -3266,14 +3274,14 @@
       <c r="C6" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="109"/>
-      <c r="E6" s="108" t="s">
+      <c r="D6" s="111"/>
+      <c r="E6" s="109" t="s">
         <v>46</v>
       </c>
       <c r="F6" s="80"/>
       <c r="G6" s="110"/>
       <c r="H6" s="110"/>
-      <c r="I6" s="109"/>
+      <c r="I6" s="111"/>
       <c r="J6" s="70" t="s">
         <v>79</v>
       </c>
@@ -3339,13 +3347,13 @@
       <c r="C8" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="108" t="s">
+      <c r="D8" s="109" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="110"/>
       <c r="F8" s="80"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
       <c r="I8" s="70" t="s">
         <v>70</v>
       </c>
@@ -3366,19 +3374,19 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="69"/>
-      <c r="C9" s="111" t="s">
+      <c r="C9" s="108" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="110"/>
-      <c r="E9" s="109"/>
+      <c r="E9" s="111"/>
       <c r="F9" s="80"/>
       <c r="G9" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="108" t="s">
+      <c r="H9" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="108" t="s">
+      <c r="I9" s="109" t="s">
         <v>71</v>
       </c>
       <c r="J9" s="70" t="s">
@@ -3398,18 +3406,18 @@
         <v>0.5</v>
       </c>
       <c r="B10" s="69"/>
-      <c r="C10" s="111"/>
+      <c r="C10" s="108"/>
       <c r="D10" s="110"/>
-      <c r="E10" s="108" t="s">
+      <c r="E10" s="109" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="80"/>
-      <c r="G10" s="108" t="s">
+      <c r="G10" s="109" t="s">
         <v>48</v>
       </c>
       <c r="H10" s="110"/>
       <c r="I10" s="110"/>
-      <c r="J10" s="108" t="s">
+      <c r="J10" s="109" t="s">
         <v>82</v>
       </c>
       <c r="K10" s="63"/>
@@ -3430,9 +3438,9 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B11" s="69"/>
-      <c r="C11" s="111"/>
+      <c r="C11" s="108"/>
       <c r="D11" s="110"/>
-      <c r="E11" s="109"/>
+      <c r="E11" s="111"/>
       <c r="F11" s="80"/>
       <c r="G11" s="110"/>
       <c r="H11" s="110"/>
@@ -3458,18 +3466,18 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="B12" s="69"/>
-      <c r="C12" s="111" t="s">
+      <c r="C12" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="109"/>
+      <c r="D12" s="111"/>
       <c r="E12" s="69" t="s">
         <v>46</v>
       </c>
       <c r="F12" s="80"/>
-      <c r="G12" s="109"/>
+      <c r="G12" s="111"/>
       <c r="H12" s="110"/>
       <c r="I12" s="110"/>
-      <c r="J12" s="109"/>
+      <c r="J12" s="111"/>
       <c r="K12" s="63"/>
       <c r="L12" s="107" t="s">
         <v>15</v>
@@ -3487,8 +3495,8 @@
         <v>0.5625</v>
       </c>
       <c r="B13" s="69"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="108" t="s">
+      <c r="C13" s="108"/>
+      <c r="D13" s="109" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="69" t="s">
@@ -3498,7 +3506,7 @@
       <c r="G13" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="109"/>
+      <c r="H13" s="111"/>
       <c r="I13" s="110"/>
       <c r="J13" s="70" t="s">
         <v>84</v>
@@ -3518,22 +3526,22 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="B14" s="69"/>
-      <c r="C14" s="111" t="s">
+      <c r="C14" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="109"/>
-      <c r="E14" s="108" t="s">
+      <c r="D14" s="111"/>
+      <c r="E14" s="109" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="80"/>
       <c r="G14" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="108" t="s">
+      <c r="H14" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="109"/>
-      <c r="J14" s="108" t="s">
+      <c r="I14" s="111"/>
+      <c r="J14" s="109" t="s">
         <v>15</v>
       </c>
       <c r="K14" s="63"/>
@@ -3554,20 +3562,20 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B15" s="69"/>
-      <c r="C15" s="111"/>
-      <c r="D15" s="108" t="s">
+      <c r="C15" s="108"/>
+      <c r="D15" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="109"/>
+      <c r="E15" s="111"/>
       <c r="F15" s="80"/>
-      <c r="G15" s="108" t="s">
+      <c r="G15" s="109" t="s">
         <v>56</v>
       </c>
       <c r="H15" s="110"/>
       <c r="I15" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="109"/>
+      <c r="J15" s="111"/>
       <c r="K15" s="63"/>
       <c r="L15" s="107"/>
       <c r="M15" s="107"/>
@@ -3582,17 +3590,17 @@
         <v>0.625</v>
       </c>
       <c r="B16" s="69"/>
-      <c r="C16" s="111" t="s">
+      <c r="C16" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="109"/>
-      <c r="E16" s="108" t="s">
+      <c r="D16" s="111"/>
+      <c r="E16" s="109" t="s">
         <v>48</v>
       </c>
       <c r="F16" s="80"/>
       <c r="G16" s="110"/>
-      <c r="H16" s="109"/>
-      <c r="I16" s="108" t="s">
+      <c r="H16" s="111"/>
+      <c r="I16" s="109" t="s">
         <v>72</v>
       </c>
       <c r="J16" s="70" t="s">
@@ -3615,18 +3623,18 @@
         <v>0.64583333333333404</v>
       </c>
       <c r="B17" s="69"/>
-      <c r="C17" s="111"/>
-      <c r="D17" s="108" t="s">
+      <c r="C17" s="108"/>
+      <c r="D17" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="109"/>
+      <c r="E17" s="111"/>
       <c r="F17" s="80"/>
       <c r="G17" s="110"/>
-      <c r="H17" s="108" t="s">
+      <c r="H17" s="109" t="s">
         <v>56</v>
       </c>
       <c r="I17" s="110"/>
-      <c r="J17" s="108" t="s">
+      <c r="J17" s="109" t="s">
         <v>86</v>
       </c>
       <c r="K17" s="63"/>
@@ -3643,15 +3651,15 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B18" s="69"/>
-      <c r="C18" s="111"/>
-      <c r="D18" s="109"/>
+      <c r="C18" s="108"/>
+      <c r="D18" s="111"/>
       <c r="E18" s="69" t="s">
         <v>21</v>
       </c>
       <c r="F18" s="80"/>
       <c r="G18" s="110"/>
       <c r="H18" s="110"/>
-      <c r="I18" s="109"/>
+      <c r="I18" s="111"/>
       <c r="J18" s="110"/>
       <c r="K18" s="63"/>
       <c r="L18" s="107"/>
@@ -3677,13 +3685,13 @@
       <c r="D19" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="108" t="s">
+      <c r="E19" s="109" t="s">
         <v>48</v>
       </c>
       <c r="F19" s="80"/>
       <c r="G19" s="110"/>
       <c r="H19" s="110"/>
-      <c r="I19" s="108" t="s">
+      <c r="I19" s="109" t="s">
         <v>73</v>
       </c>
       <c r="J19" s="110"/>
@@ -3705,14 +3713,14 @@
       <c r="C20" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="108" t="s">
+      <c r="D20" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="109"/>
+      <c r="E20" s="111"/>
       <c r="F20" s="80"/>
       <c r="G20" s="110"/>
       <c r="H20" s="110"/>
-      <c r="I20" s="109"/>
+      <c r="I20" s="111"/>
       <c r="J20" s="110"/>
       <c r="K20" s="63"/>
       <c r="L20" s="94" t="s">
@@ -3732,20 +3740,20 @@
         <v>0.72916666666666696</v>
       </c>
       <c r="B21" s="69"/>
-      <c r="C21" s="111" t="s">
+      <c r="C21" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="109"/>
+      <c r="D21" s="111"/>
       <c r="E21" s="69" t="s">
         <v>36</v>
       </c>
       <c r="F21" s="80"/>
       <c r="G21" s="110"/>
-      <c r="H21" s="109"/>
-      <c r="I21" s="108" t="s">
+      <c r="H21" s="111"/>
+      <c r="I21" s="109" t="s">
         <v>70</v>
       </c>
-      <c r="J21" s="109"/>
+      <c r="J21" s="111"/>
       <c r="K21" s="63"/>
       <c r="L21" s="107" t="s">
         <v>91</v>
@@ -3762,7 +3770,7 @@
         <v>0.75</v>
       </c>
       <c r="B22" s="69"/>
-      <c r="C22" s="111"/>
+      <c r="C22" s="108"/>
       <c r="D22" s="69" t="s">
         <v>37</v>
       </c>
@@ -3772,7 +3780,7 @@
       <c r="H22" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="109"/>
+      <c r="I22" s="111"/>
       <c r="J22" s="70" t="s">
         <v>87</v>
       </c>
@@ -3793,17 +3801,17 @@
         <v>0.77083333333333404</v>
       </c>
       <c r="B23" s="69"/>
-      <c r="C23" s="111"/>
+      <c r="C23" s="108"/>
       <c r="D23" s="69" t="s">
         <v>36</v>
       </c>
       <c r="E23" s="62"/>
       <c r="F23" s="80"/>
-      <c r="G23" s="109"/>
+      <c r="G23" s="111"/>
       <c r="H23" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="I23" s="108" t="s">
+      <c r="I23" s="109" t="s">
         <v>74</v>
       </c>
       <c r="J23" s="62"/>
@@ -3831,7 +3839,7 @@
       <c r="F24" s="80"/>
       <c r="G24" s="62"/>
       <c r="H24" s="62"/>
-      <c r="I24" s="109"/>
+      <c r="I24" s="111"/>
       <c r="J24" s="62"/>
       <c r="K24" s="63"/>
       <c r="L24" s="94" t="s">
@@ -3965,6 +3973,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="S6:S9"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="O7:O9"/>
+    <mergeCell ref="O11:O17"/>
+    <mergeCell ref="O18:O20"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="M6:M10"/>
+    <mergeCell ref="M12:M17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="L14:L19"/>
+    <mergeCell ref="L21:L23"/>
+    <mergeCell ref="L5:L11"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="N5:N10"/>
+    <mergeCell ref="H9:H13"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="H17:H21"/>
+    <mergeCell ref="N13:N18"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="H5:H8"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="G4:G8"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
     <mergeCell ref="W14:W16"/>
     <mergeCell ref="V16:V18"/>
     <mergeCell ref="C16:C18"/>
@@ -3981,40 +4023,6 @@
     <mergeCell ref="G10:G12"/>
     <mergeCell ref="G15:G23"/>
     <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="G4:G8"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="N5:N10"/>
-    <mergeCell ref="H9:H13"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="H17:H21"/>
-    <mergeCell ref="N13:N18"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="H5:H8"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="M6:M10"/>
-    <mergeCell ref="M12:M17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="L14:L19"/>
-    <mergeCell ref="L21:L23"/>
-    <mergeCell ref="L5:L11"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="S6:S9"/>
-    <mergeCell ref="Q10:Q11"/>
-    <mergeCell ref="O7:O9"/>
-    <mergeCell ref="O11:O17"/>
-    <mergeCell ref="O18:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>